<commit_message>
Pushing new KPI Sorter Reasons
</commit_message>
<xml_diff>
--- a/Tutor_Concerns.xlsx
+++ b/Tutor_Concerns.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tyler_harrington2/Desktop/FL_Dashboards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FFF247BC-9802-8242-895C-BAC973EC2E8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E0E97A2B-DF18-0041-8DDB-914C22B5E137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{92DEE1D6-509C-344A-AA8F-D8DD2317BD81}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14860" xr2:uid="{92DEE1D6-509C-344A-AA8F-D8DD2317BD81}"/>
   </bookViews>
   <sheets>
     <sheet name="Concerns" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="2465" uniqueCount="453">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="3309" uniqueCount="525">
   <si>
     <t>Tutor Name</t>
   </si>
@@ -1395,6 +1395,222 @@
   </si>
   <si>
     <t>8/10/25 - 9/6/25</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; Prep Time % &gt; 15%; Diff M2M Prep Time % &gt; 10%; Diff M2M % to Delivery Target &lt; -20% and % to Delivery Target &lt; 85%; Diff M2M % to Availability Target &lt; -10% and % to Availability Target &lt; 95%</t>
+  </si>
+  <si>
+    <t>% Parent Updates &lt; 85%; Ratio of PPW Events with Attached PPW &lt; 1/2; Avg. NPS Score &lt; 8</t>
+  </si>
+  <si>
+    <t>% Parent Updates &lt; 90%; % Sessions on Time &lt; 90%; Prep Time % &gt; 15%; Diff M2M % to Delivery Target &lt; -20% and % to Delivery Target &lt; 85%; Diff M2M % to Availability Target &lt; -10% and % to Availability Target &lt; 95%</t>
+  </si>
+  <si>
+    <t>% Parent Updates &lt; 90%; % of Active Students with Progress Updates Completed in last 2 months &lt; 70%; Diff M2M Prep Time % &gt; 10%</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; Prep Time % &gt; 15%; Diff M2M Prep Time % &gt; 10%; Diff M2M % to Availability Target &lt; -10% and % to Availability Target &lt; 95%</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; Diff M2M % to Availability Target &lt; -10% and % to Availability Target &lt; 95%</t>
+  </si>
+  <si>
+    <t>% Parent Updates &lt; 90%; Diff M2M % to Delivery Target &lt; -20% and % to Delivery Target &lt; 85%</t>
+  </si>
+  <si>
+    <t>% Parent Updates &lt; 90%; % of Active Students with Progress Updates Completed in last 2 months &lt; 70%; Prep Time % &gt; 15%</t>
+  </si>
+  <si>
+    <t>Ben Chamberlain</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; % Parent Updates &lt; 85%; Prep Time % &gt; 15%; Bottom 10% in % to Delivery Target for tier</t>
+  </si>
+  <si>
+    <t>Ratio of PPW Events with Attached PPW &lt; 1/2; % of Active Students with Progress Updates Completed in last 2 months &lt; 50%; Prep Time % &gt; 15%; Diff M2M % to Delivery Target &lt; -20% and % to Delivery Target &lt; 85%</t>
+  </si>
+  <si>
+    <t>Ratio of PPW Events with Attached PPW &lt; 1/2; % of Active Students with Progress Updates Completed in last 2 months &lt; 50%; Weighted Repurchases = 0; Prep Time % &gt; 15%</t>
+  </si>
+  <si>
+    <t>Brock Dilley</t>
+  </si>
+  <si>
+    <t>% Parent Updates &lt; 90%; Weighted Repurchases = 0; Prep Time % &gt; 15%; Diff M2M Prep Time % &gt; 10%; Avg. NPS Score &lt; 8</t>
+  </si>
+  <si>
+    <t>Prep Time % &gt; 15%; Diff M2M Prep Time % &gt; 10%; Bottom 10% in % to Delivery Target for tier</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; Prep Time % &gt; 15%; Diff M2M % to Availability Target &lt; -10% and % to Availability Target &lt; 95%</t>
+  </si>
+  <si>
+    <t>Cayden Koselak</t>
+  </si>
+  <si>
+    <t>% Sessions on Time &lt; 90%; Ratio of PPW Events with Attached PPW &lt; 1/2; % of Active Students with Progress Updates Completed in last 2 months &lt; 70%; Prep Time % &gt; 15%</t>
+  </si>
+  <si>
+    <t>Christelle Rocha</t>
+  </si>
+  <si>
+    <t>% of Active Students with Progress Updates Completed in last 2 months &lt; 70%; Prep Time % &gt; 15%; Diff M2M Prep Time % &gt; 10%</t>
+  </si>
+  <si>
+    <t>% Sessions on Time &lt; 90%; % of Active Students with Progress Updates Completed in last 2 months &lt; 70%; Prep Time % &gt; 15%</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; % Parent Updates &lt; 85%; Diff M2M % to Delivery Target &lt; -20% and % to Delivery Target &lt; 85%; Diff M2M % to Availability Target &lt; -10% and % to Availability Target &lt; 95%</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; Prep Time % &gt; 15%; Diff M2M Prep Time % &gt; 10%</t>
+  </si>
+  <si>
+    <t>% Parent Updates &lt; 90%; Prep Time % &gt; 15%; Diff M2M % to Delivery Target &lt; -20% and % to Delivery Target &lt; 85%</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; Ratio of PPW Events with Attached PPW &lt; 1/2; Prep Time % &gt; 15%; Diff M2M % to Availability Target &lt; -10% and % to Availability Target &lt; 95%</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; Ratio of PPW Events with Attached PPW &lt; 1/2; % of Active Students with Progress Updates Completed in last 2 months &lt; 50%; Diff M2M % of Active Students with Progress Updates Completed in last 2 months &lt; -20%; Diff M2M % to Availability Target &lt; -10% and % to Availability Target &lt; 95%</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; % of Active Students with Progress Updates Completed in last 2 months &lt; 70%; Diff M2M % of Active Students with Progress Updates Completed in last 2 months &lt; -20%; Prep Time % &gt; 15%; Diff M2M % to Delivery Target &lt; -20% and % to Delivery Target &lt; 85%; Diff M2M % to Availability Target &lt; -10% and % to Availability Target &lt; 95%</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; % Parent Updates &lt; 85%; Ratio of PPW Events with Attached PPW &lt; 1/2; Prep Time % &gt; 15%; Diff M2M Prep Time % &gt; 10%; Bottom 10% in % to Delivery Target for tier</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; % of Active Students with Progress Updates Completed in last 2 months &lt; 50%; Prep Time % &gt; 15%; Diff M2M % to Delivery Target &lt; -20% and % to Delivery Target &lt; 85%; Diff M2M % to Availability Target &lt; -10% and % to Availability Target &lt; 95%</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; % Parent Updates &lt; 85%; % of Active Students with Progress Updates Completed in last 2 months &lt; 60%; Diff M2M % of Active Students with Progress Updates Completed in last 2 months &lt; -20%; Diff M2M % to Delivery Target &lt; -20% and % to Delivery Target &lt; 85%; Diff M2M % to Availability Target &lt; -10% and % to Availability Target &lt; 95%; Bottom 10% in % to Delivery Target for tier</t>
+  </si>
+  <si>
+    <t>Ratio of PPW Events with Attached PPW &lt; 1/2; % of Active Students with Progress Updates Completed in last 2 months &lt; 50%; Diff M2M % to Delivery Target &lt; -20% and % to Delivery Target &lt; 85%; Diff M2M % to Availability Target &lt; -10% and % to Availability Target &lt; 95%; Bottom 10% in % to Delivery Target for tier</t>
+  </si>
+  <si>
+    <t>% of Active Students with Progress Updates Completed in last 2 months &lt; 50%; Prep Time % &gt; 15%; Diff M2M Prep Time % &gt; 10%; Bottom 10% in % to Delivery Target for tier</t>
+  </si>
+  <si>
+    <t>Jill Watson</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; % Parent Updates &lt; 90%; Ratio of PPW Events with Attached PPW &lt; 1/2; Prep Time % &gt; 15%; Bottom 10% in % to Delivery Target for tier</t>
+  </si>
+  <si>
+    <t>% Sessions on Time &lt; 85%; Ratio of PPW Events with Attached PPW &lt; 1/2; % of Active Students with Progress Updates Completed in last 2 months &lt; 50%; Diff M2M % of Active Students with Progress Updates Completed in last 2 months &lt; -20%; Prep Time % &gt; 15%; Diff M2M Prep Time % &gt; 10%</t>
+  </si>
+  <si>
+    <t>Ratio of PPW Events with Attached PPW &lt; 1/2; Prep Time % &gt; 15%; Diff M2M % to Delivery Target &lt; -20% and % to Delivery Target &lt; 85%</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; % Parent Updates &lt; 85%; Ratio of PPW Events with Attached PPW &lt; 1/2; Prep Time % &gt; 15%; Diff M2M % to Delivery Target &lt; -20% and % to Delivery Target &lt; 85%; Diff M2M % to Availability Target &lt; -10% and % to Availability Target &lt; 95%</t>
+  </si>
+  <si>
+    <t>Prep Time % &gt; 15%; Diff M2M % to Delivery Target &lt; -20% and % to Delivery Target &lt; 85%; Bottom 10% in % to Delivery Target for tier</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; % of Active Students with Progress Updates Completed in last 2 months &lt; 60%; Diff M2M % to Availability Target &lt; -10% and % to Availability Target &lt; 95%; Bottom 10% in % to Delivery Target for tier</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; Prep Time % &gt; 15%; Diff M2M Prep Time % &gt; 10%; Bottom 10% in % to Delivery Target for tier</t>
+  </si>
+  <si>
+    <t>Lauren Seidl</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; % Parent Updates &lt; 85%; Prep Time % &gt; 15%; Diff M2M Prep Time % &gt; 10%</t>
+  </si>
+  <si>
+    <t>% Parent Updates &lt; 85%; Prep Time % &gt; 15%; Diff M2M Prep Time % &gt; 10%; Bottom 10% in % to Delivery Target for tier</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; % of Active Students with Progress Updates Completed in last 2 months &lt; 60%; Diff M2M Prep Time % &gt; 10%; Bottom 10% in % to Delivery Target for tier</t>
+  </si>
+  <si>
+    <t>Prep Time % &gt; 15%; Diff M2M % to Delivery Target &lt; -20% and % to Delivery Target &lt; 85%; Diff M2M % to Availability Target &lt; -10% and % to Availability Target &lt; 95%</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; % of Active Students with Progress Updates Completed in last 2 months &lt; 50%; Prep Time % &gt; 15%; Diff M2M Prep Time % &gt; 10%; Bottom 10% in % to Delivery Target for tier</t>
+  </si>
+  <si>
+    <t>% Parent Updates &lt; 85%; Ratio of PPW Events with Attached PPW &lt; 1/2; % of Active Students with Progress Updates Completed in last 2 months &lt; 50%; Prep Time % &gt; 15%; Diff M2M Prep Time % &gt; 10%</t>
+  </si>
+  <si>
+    <t>% Sessions on Time &lt; 85%; Ratio of PPW Events with Attached PPW &lt; 1/2; % of Active Students with Progress Updates Completed in last 2 months &lt; 50%; Prep Time % &gt; 15%</t>
+  </si>
+  <si>
+    <t>% of Active Students with Progress Updates Completed in last 2 months &lt; 50%; Diff M2M % of Active Students with Progress Updates Completed in last 2 months &lt; -20%; Diff M2M % to Delivery Target &lt; -20% and % to Delivery Target &lt; 85%; Bottom 10% in % to Delivery Target for tier</t>
+  </si>
+  <si>
+    <t>Ratio of PPW Events with Attached PPW &lt; 1/2; Prep Time % &gt; 15%; Diff M2M Prep Time % &gt; 10%; Avg. NPS Score &lt; 8</t>
+  </si>
+  <si>
+    <t>% Sessions on Time &lt; 90%; % of Active Students with Progress Updates Completed in last 2 months &lt; 60%; Prep Time % &gt; 15%</t>
+  </si>
+  <si>
+    <t>Ratio of PPW Events with Attached PPW &lt; 1/2; % of Active Students with Progress Updates Completed in last 2 months &lt; 70%; Diff M2M % to Availability Target &lt; -10% and % to Availability Target &lt; 95%</t>
+  </si>
+  <si>
+    <t>% Parent Updates &lt; 90%; % Sessions on Time &lt; 85%; Prep Time % &gt; 15%</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; Prep Time % &gt; 15%</t>
+  </si>
+  <si>
+    <t>Ratio of PPW Events with Attached PPW &lt; 1/2; % of Active Students with Progress Updates Completed in last 2 months &lt; 70%; Diff M2M % of Active Students with Progress Updates Completed in last 2 months &lt; -20%</t>
+  </si>
+  <si>
+    <t>Ratio of PPW Events with Attached PPW &lt; 1/2; % of Active Students with Progress Updates Completed in last 2 months &lt; 60%; Diff M2M % of Active Students with Progress Updates Completed in last 2 months &lt; -20%</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; % Parent Updates &lt; 85%; Ratio of PPW Events with Attached PPW &lt; 1/2; % of Active Students with Progress Updates Completed in last 2 months &lt; 50%; Diff M2M % of Active Students with Progress Updates Completed in last 2 months &lt; -20%; Diff M2M % to Availability Target &lt; -10% and % to Availability Target &lt; 95%</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; Ratio of PPW Events with Attached PPW &lt; 1/2; Diff M2M % to Availability Target &lt; -10% and % to Availability Target &lt; 95%</t>
+  </si>
+  <si>
+    <t>% Parent Updates &lt; 90%; Ratio of PPW Events with Attached PPW &lt; 1/2; Prep Time % &gt; 15%; Diff M2M % to Delivery Target &lt; -20% and % to Delivery Target &lt; 85%</t>
+  </si>
+  <si>
+    <t>Silvester Harrison</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; % Parent Updates &lt; 85%; Diff M2M % of Active Students with Progress Updates Completed in last 2 months &lt; -20%; Diff M2M % to Delivery Target &lt; -20% and % to Delivery Target &lt; 85%; Diff M2M % to Availability Target &lt; -10% and % to Availability Target &lt; 95%</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; % Parent Updates &lt; 85%; Ratio of PPW Events with Attached PPW &lt; 1/2; % of Active Students with Progress Updates Completed in last 2 months &lt; 70%; Prep Time % &gt; 15%; Diff M2M Prep Time % &gt; 10%; Diff M2M % to Availability Target &lt; -10% and % to Availability Target &lt; 95%</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; Diff M2M % to Delivery Target &lt; -20% and % to Delivery Target &lt; 85%; Diff M2M % to Availability Target &lt; -10% and % to Availability Target &lt; 95%</t>
+  </si>
+  <si>
+    <t>% Parent Updates &lt; 90%; Ratio of PPW Events with Attached PPW &lt; 1/2; % of Active Students with Progress Updates Completed in last 2 months &lt; 60%; Diff M2M % of Active Students with Progress Updates Completed in last 2 months &lt; -20%; Prep Time % &gt; 15%</t>
+  </si>
+  <si>
+    <t>% Parent Updates &lt; 90%; Ratio of PPW Events with Attached PPW &lt; 1/2; % of Active Students with Progress Updates Completed in last 2 months &lt; 50%; Prep Time % &gt; 15%; Diff M2M Prep Time % &gt; 10%</t>
+  </si>
+  <si>
+    <t>% of Active Students with Progress Updates Completed in last 2 months &lt; 70%; Prep Time % &gt; 15%; Diff M2M % to Delivery Target &lt; -20% and % to Delivery Target &lt; 85%; Bottom 10% in % to Delivery Target for tier</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; % Parent Updates &lt; 85%; Ratio of PPW Events with Attached PPW &lt; 1/2; % of Active Students with Progress Updates Completed in last 2 months &lt; 50%; Diff M2M % to Availability Target &lt; -10% and % to Availability Target &lt; 95%</t>
+  </si>
+  <si>
+    <t>% Sessions on Time &lt; 85%; Diff M2M % of Active Students with Progress Updates Completed in last 2 months &lt; -20%; Prep Time % &gt; 15%</t>
+  </si>
+  <si>
+    <t>Zach McFatridge</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; % Parent Updates &lt; 90%; % of Active Students with Progress Updates Completed in last 2 months &lt; 50%; Diff M2M % of Active Students with Progress Updates Completed in last 2 months &lt; -20%</t>
+  </si>
+  <si>
+    <t>% of Active Students with Progress Updates Completed in last 2 months &lt; 60%; Prep Time % &gt; 15%; Diff M2M % to Availability Target &lt; -10% and % to Availability Target &lt; 95%</t>
+  </si>
+  <si>
+    <t>11/2/25 - 11/30/25</t>
   </si>
 </sst>
 </file>
@@ -2264,10 +2480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDA4CB91-83C8-694D-BBCD-170E9881DA10}">
-  <dimension ref="A1:E616"/>
+  <dimension ref="A1:E827"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" topLeftCell="A504" workbookViewId="0">
+      <selection activeCell="D614" sqref="D614"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12747,6 +12963,3593 @@
         <v>6</v>
       </c>
     </row>
+    <row r="617" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A617" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B617" t="s">
+        <v>4</v>
+      </c>
+      <c r="C617" t="s">
+        <v>5</v>
+      </c>
+      <c r="D617">
+        <v>3</v>
+      </c>
+      <c r="E617" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="618" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A618" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B618" t="s">
+        <v>7</v>
+      </c>
+      <c r="C618" t="s">
+        <v>5</v>
+      </c>
+      <c r="D618">
+        <v>2</v>
+      </c>
+      <c r="E618" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="619" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A619" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B619" t="s">
+        <v>8</v>
+      </c>
+      <c r="C619" t="s">
+        <v>9</v>
+      </c>
+      <c r="D619">
+        <v>2</v>
+      </c>
+      <c r="E619" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="620" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A620" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B620" t="s">
+        <v>11</v>
+      </c>
+      <c r="C620" t="s">
+        <v>5</v>
+      </c>
+      <c r="D620">
+        <v>1</v>
+      </c>
+      <c r="E620" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="621" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A621" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B621" t="s">
+        <v>13</v>
+      </c>
+      <c r="C621" t="s">
+        <v>14</v>
+      </c>
+      <c r="D621">
+        <v>5</v>
+      </c>
+      <c r="E621" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="622" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A622" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B622" t="s">
+        <v>16</v>
+      </c>
+      <c r="C622" t="s">
+        <v>5</v>
+      </c>
+      <c r="D622">
+        <v>5</v>
+      </c>
+      <c r="E622" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="623" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A623" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B623" t="s">
+        <v>18</v>
+      </c>
+      <c r="C623" t="s">
+        <v>19</v>
+      </c>
+      <c r="D623">
+        <v>3</v>
+      </c>
+      <c r="E623" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="624" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A624" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B624" t="s">
+        <v>21</v>
+      </c>
+      <c r="C624" t="s">
+        <v>14</v>
+      </c>
+      <c r="D624">
+        <v>2</v>
+      </c>
+      <c r="E624" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="625" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A625" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B625" t="s">
+        <v>23</v>
+      </c>
+      <c r="C625" t="s">
+        <v>24</v>
+      </c>
+      <c r="D625">
+        <v>4</v>
+      </c>
+      <c r="E625" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="626" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A626" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B626" t="s">
+        <v>26</v>
+      </c>
+      <c r="C626" t="s">
+        <v>27</v>
+      </c>
+      <c r="D626">
+        <v>5</v>
+      </c>
+      <c r="E626" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="627" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A627" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B627" t="s">
+        <v>29</v>
+      </c>
+      <c r="C627" t="s">
+        <v>14</v>
+      </c>
+      <c r="D627">
+        <v>5</v>
+      </c>
+      <c r="E627" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="628" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A628" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B628" t="s">
+        <v>31</v>
+      </c>
+      <c r="C628" t="s">
+        <v>5</v>
+      </c>
+      <c r="D628">
+        <v>5</v>
+      </c>
+      <c r="E628" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="629" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A629" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B629" t="s">
+        <v>33</v>
+      </c>
+      <c r="C629" t="s">
+        <v>5</v>
+      </c>
+      <c r="D629">
+        <v>4</v>
+      </c>
+      <c r="E629" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="630" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A630" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B630" t="s">
+        <v>35</v>
+      </c>
+      <c r="C630" t="s">
+        <v>27</v>
+      </c>
+      <c r="D630">
+        <v>3</v>
+      </c>
+      <c r="E630" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="631" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A631" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B631" t="s">
+        <v>37</v>
+      </c>
+      <c r="C631" t="s">
+        <v>14</v>
+      </c>
+      <c r="D631">
+        <v>3</v>
+      </c>
+      <c r="E631" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="632" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A632" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B632" t="s">
+        <v>39</v>
+      </c>
+      <c r="C632" t="s">
+        <v>5</v>
+      </c>
+      <c r="D632">
+        <v>2</v>
+      </c>
+      <c r="E632" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="633" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A633" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B633" t="s">
+        <v>40</v>
+      </c>
+      <c r="C633" t="s">
+        <v>14</v>
+      </c>
+      <c r="D633">
+        <v>5</v>
+      </c>
+      <c r="E633" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="634" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A634" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B634" t="s">
+        <v>41</v>
+      </c>
+      <c r="C634" t="s">
+        <v>9</v>
+      </c>
+      <c r="D634">
+        <v>5</v>
+      </c>
+      <c r="E634" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="635" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A635" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B635" t="s">
+        <v>43</v>
+      </c>
+      <c r="C635" t="s">
+        <v>19</v>
+      </c>
+      <c r="D635">
+        <v>4</v>
+      </c>
+      <c r="E635" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="636" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A636" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B636" t="s">
+        <v>45</v>
+      </c>
+      <c r="C636" t="s">
+        <v>24</v>
+      </c>
+      <c r="D636">
+        <v>4</v>
+      </c>
+      <c r="E636" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="637" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A637" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B637" t="s">
+        <v>461</v>
+      </c>
+      <c r="C637" t="s">
+        <v>51</v>
+      </c>
+      <c r="D637">
+        <v>5</v>
+      </c>
+      <c r="E637" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="638" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A638" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B638" t="s">
+        <v>47</v>
+      </c>
+      <c r="C638" t="s">
+        <v>27</v>
+      </c>
+      <c r="D638">
+        <v>1</v>
+      </c>
+      <c r="E638" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="639" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A639" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B639" t="s">
+        <v>48</v>
+      </c>
+      <c r="C639" t="s">
+        <v>24</v>
+      </c>
+      <c r="D639">
+        <v>5</v>
+      </c>
+      <c r="E639" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="640" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A640" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B640" t="s">
+        <v>50</v>
+      </c>
+      <c r="C640" t="s">
+        <v>24</v>
+      </c>
+      <c r="D640">
+        <v>5</v>
+      </c>
+      <c r="E640" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="641" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A641" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B641" t="s">
+        <v>53</v>
+      </c>
+      <c r="C641" t="s">
+        <v>24</v>
+      </c>
+      <c r="D641">
+        <v>2</v>
+      </c>
+      <c r="E641" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="642" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A642" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B642" t="s">
+        <v>55</v>
+      </c>
+      <c r="C642" t="s">
+        <v>27</v>
+      </c>
+      <c r="D642">
+        <v>2</v>
+      </c>
+      <c r="E642" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="643" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A643" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B643" t="s">
+        <v>57</v>
+      </c>
+      <c r="C643" t="s">
+        <v>24</v>
+      </c>
+      <c r="D643">
+        <v>1</v>
+      </c>
+      <c r="E643" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="644" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A644" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B644" t="s">
+        <v>465</v>
+      </c>
+      <c r="C644" t="s">
+        <v>51</v>
+      </c>
+      <c r="D644">
+        <v>1</v>
+      </c>
+      <c r="E644" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="645" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A645" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B645" t="s">
+        <v>58</v>
+      </c>
+      <c r="C645" t="s">
+        <v>27</v>
+      </c>
+      <c r="D645">
+        <v>4</v>
+      </c>
+      <c r="E645" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="646" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A646" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B646" t="s">
+        <v>59</v>
+      </c>
+      <c r="C646" t="s">
+        <v>9</v>
+      </c>
+      <c r="D646">
+        <v>1</v>
+      </c>
+      <c r="E646" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="647" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A647" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B647" t="s">
+        <v>61</v>
+      </c>
+      <c r="C647" t="s">
+        <v>62</v>
+      </c>
+      <c r="D647">
+        <v>3</v>
+      </c>
+      <c r="E647" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="648" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A648" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B648" t="s">
+        <v>64</v>
+      </c>
+      <c r="C648" t="s">
+        <v>14</v>
+      </c>
+      <c r="D648">
+        <v>1</v>
+      </c>
+      <c r="E648" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="649" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A649" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B649" t="s">
+        <v>65</v>
+      </c>
+      <c r="C649" t="s">
+        <v>5</v>
+      </c>
+      <c r="D649">
+        <v>4</v>
+      </c>
+      <c r="E649" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="650" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A650" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B650" t="s">
+        <v>67</v>
+      </c>
+      <c r="C650" t="s">
+        <v>14</v>
+      </c>
+      <c r="D650">
+        <v>1</v>
+      </c>
+      <c r="E650" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="651" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A651" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B651" t="s">
+        <v>69</v>
+      </c>
+      <c r="C651" t="s">
+        <v>9</v>
+      </c>
+      <c r="D651">
+        <v>3</v>
+      </c>
+      <c r="E651" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="652" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A652" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B652" t="s">
+        <v>469</v>
+      </c>
+      <c r="C652" t="s">
+        <v>62</v>
+      </c>
+      <c r="D652">
+        <v>1</v>
+      </c>
+      <c r="E652" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="653" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A653" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B653" t="s">
+        <v>70</v>
+      </c>
+      <c r="C653" t="s">
+        <v>9</v>
+      </c>
+      <c r="D653">
+        <v>2</v>
+      </c>
+      <c r="E653" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="654" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A654" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B654" t="s">
+        <v>71</v>
+      </c>
+      <c r="C654" t="s">
+        <v>24</v>
+      </c>
+      <c r="D654">
+        <v>2</v>
+      </c>
+      <c r="E654" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="655" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A655" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B655" t="s">
+        <v>73</v>
+      </c>
+      <c r="C655" t="s">
+        <v>5</v>
+      </c>
+      <c r="D655">
+        <v>4</v>
+      </c>
+      <c r="E655" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="656" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A656" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B656" t="s">
+        <v>75</v>
+      </c>
+      <c r="C656" t="s">
+        <v>14</v>
+      </c>
+      <c r="D656">
+        <v>3</v>
+      </c>
+      <c r="E656" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="657" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A657" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B657" t="s">
+        <v>76</v>
+      </c>
+      <c r="C657" t="s">
+        <v>24</v>
+      </c>
+      <c r="D657">
+        <v>2</v>
+      </c>
+      <c r="E657" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="658" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A658" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B658" t="s">
+        <v>471</v>
+      </c>
+      <c r="C658" t="s">
+        <v>62</v>
+      </c>
+      <c r="D658">
+        <v>3</v>
+      </c>
+      <c r="E658" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="659" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A659" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B659" t="s">
+        <v>78</v>
+      </c>
+      <c r="C659" t="s">
+        <v>27</v>
+      </c>
+      <c r="D659">
+        <v>1</v>
+      </c>
+      <c r="E659" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="660" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A660" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B660" t="s">
+        <v>79</v>
+      </c>
+      <c r="C660" t="s">
+        <v>14</v>
+      </c>
+      <c r="D660">
+        <v>3</v>
+      </c>
+      <c r="E660" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="661" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A661" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B661" t="s">
+        <v>80</v>
+      </c>
+      <c r="C661" t="s">
+        <v>27</v>
+      </c>
+      <c r="D661">
+        <v>4</v>
+      </c>
+      <c r="E661" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="662" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A662" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B662" t="s">
+        <v>82</v>
+      </c>
+      <c r="C662" t="s">
+        <v>9</v>
+      </c>
+      <c r="D662">
+        <v>4</v>
+      </c>
+      <c r="E662" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="663" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A663" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B663" t="s">
+        <v>84</v>
+      </c>
+      <c r="C663" t="s">
+        <v>9</v>
+      </c>
+      <c r="D663">
+        <v>5</v>
+      </c>
+      <c r="E663" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="664" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A664" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B664" t="s">
+        <v>86</v>
+      </c>
+      <c r="C664" t="s">
+        <v>9</v>
+      </c>
+      <c r="D664">
+        <v>2</v>
+      </c>
+      <c r="E664" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="665" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A665" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B665" t="s">
+        <v>88</v>
+      </c>
+      <c r="C665" t="s">
+        <v>5</v>
+      </c>
+      <c r="D665">
+        <v>3</v>
+      </c>
+      <c r="E665" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="666" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A666" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B666" t="s">
+        <v>92</v>
+      </c>
+      <c r="C666" t="s">
+        <v>24</v>
+      </c>
+      <c r="D666">
+        <v>5</v>
+      </c>
+      <c r="E666" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="667" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A667" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B667" t="s">
+        <v>94</v>
+      </c>
+      <c r="C667" t="s">
+        <v>24</v>
+      </c>
+      <c r="D667">
+        <v>5</v>
+      </c>
+      <c r="E667" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="668" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A668" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B668" t="s">
+        <v>96</v>
+      </c>
+      <c r="C668" t="s">
+        <v>27</v>
+      </c>
+      <c r="D668">
+        <v>3</v>
+      </c>
+      <c r="E668" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="669" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A669" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B669" t="s">
+        <v>98</v>
+      </c>
+      <c r="C669" t="s">
+        <v>9</v>
+      </c>
+      <c r="D669">
+        <v>5</v>
+      </c>
+      <c r="E669" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="670" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A670" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B670" t="s">
+        <v>100</v>
+      </c>
+      <c r="C670" t="s">
+        <v>14</v>
+      </c>
+      <c r="D670">
+        <v>5</v>
+      </c>
+      <c r="E670" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="671" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A671" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B671" t="s">
+        <v>102</v>
+      </c>
+      <c r="C671" t="s">
+        <v>9</v>
+      </c>
+      <c r="D671">
+        <v>2</v>
+      </c>
+      <c r="E671" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="672" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A672" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B672" t="s">
+        <v>104</v>
+      </c>
+      <c r="C672" t="s">
+        <v>62</v>
+      </c>
+      <c r="D672">
+        <v>3</v>
+      </c>
+      <c r="E672" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="673" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A673" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B673" t="s">
+        <v>105</v>
+      </c>
+      <c r="C673" t="s">
+        <v>14</v>
+      </c>
+      <c r="D673">
+        <v>4</v>
+      </c>
+      <c r="E673" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="674" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A674" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B674" t="s">
+        <v>107</v>
+      </c>
+      <c r="C674" t="s">
+        <v>5</v>
+      </c>
+      <c r="D674">
+        <v>2</v>
+      </c>
+      <c r="E674" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="675" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A675" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B675" t="s">
+        <v>108</v>
+      </c>
+      <c r="C675" t="s">
+        <v>5</v>
+      </c>
+      <c r="D675">
+        <v>3</v>
+      </c>
+      <c r="E675" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="676" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A676" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B676" t="s">
+        <v>109</v>
+      </c>
+      <c r="C676" t="s">
+        <v>24</v>
+      </c>
+      <c r="D676">
+        <v>3</v>
+      </c>
+      <c r="E676" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="677" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A677" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B677" t="s">
+        <v>111</v>
+      </c>
+      <c r="C677" t="s">
+        <v>5</v>
+      </c>
+      <c r="D677">
+        <v>3</v>
+      </c>
+      <c r="E677" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="678" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A678" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B678" t="s">
+        <v>112</v>
+      </c>
+      <c r="C678" t="s">
+        <v>5</v>
+      </c>
+      <c r="D678">
+        <v>2</v>
+      </c>
+      <c r="E678" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="679" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A679" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B679" t="s">
+        <v>114</v>
+      </c>
+      <c r="C679" t="s">
+        <v>9</v>
+      </c>
+      <c r="D679">
+        <v>1</v>
+      </c>
+      <c r="E679" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="680" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A680" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B680" t="s">
+        <v>115</v>
+      </c>
+      <c r="C680" t="s">
+        <v>9</v>
+      </c>
+      <c r="D680">
+        <v>2</v>
+      </c>
+      <c r="E680" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="681" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A681" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B681" t="s">
+        <v>116</v>
+      </c>
+      <c r="C681" t="s">
+        <v>5</v>
+      </c>
+      <c r="D681">
+        <v>2</v>
+      </c>
+      <c r="E681" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="682" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A682" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B682" t="s">
+        <v>117</v>
+      </c>
+      <c r="C682" t="s">
+        <v>14</v>
+      </c>
+      <c r="D682">
+        <v>2</v>
+      </c>
+      <c r="E682" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="683" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A683" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B683" t="s">
+        <v>118</v>
+      </c>
+      <c r="C683" t="s">
+        <v>24</v>
+      </c>
+      <c r="D683">
+        <v>3</v>
+      </c>
+      <c r="E683" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="684" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A684" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B684" t="s">
+        <v>120</v>
+      </c>
+      <c r="C684" t="s">
+        <v>24</v>
+      </c>
+      <c r="D684">
+        <v>2</v>
+      </c>
+      <c r="E684" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="685" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A685" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B685" t="s">
+        <v>122</v>
+      </c>
+      <c r="C685" t="s">
+        <v>14</v>
+      </c>
+      <c r="D685">
+        <v>5</v>
+      </c>
+      <c r="E685" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="686" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A686" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B686" t="s">
+        <v>124</v>
+      </c>
+      <c r="C686" t="s">
+        <v>19</v>
+      </c>
+      <c r="D686">
+        <v>1</v>
+      </c>
+      <c r="E686" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="687" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A687" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B687" t="s">
+        <v>126</v>
+      </c>
+      <c r="C687" t="s">
+        <v>24</v>
+      </c>
+      <c r="D687">
+        <v>5</v>
+      </c>
+      <c r="E687" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="688" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A688" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B688" t="s">
+        <v>127</v>
+      </c>
+      <c r="C688" t="s">
+        <v>9</v>
+      </c>
+      <c r="D688">
+        <v>5</v>
+      </c>
+      <c r="E688" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="689" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A689" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B689" t="s">
+        <v>129</v>
+      </c>
+      <c r="C689" t="s">
+        <v>19</v>
+      </c>
+      <c r="D689">
+        <v>2</v>
+      </c>
+      <c r="E689" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="690" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A690" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B690" t="s">
+        <v>130</v>
+      </c>
+      <c r="C690" t="s">
+        <v>14</v>
+      </c>
+      <c r="D690">
+        <v>3</v>
+      </c>
+      <c r="E690" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="691" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A691" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B691" t="s">
+        <v>131</v>
+      </c>
+      <c r="C691" t="s">
+        <v>5</v>
+      </c>
+      <c r="D691">
+        <v>1</v>
+      </c>
+      <c r="E691" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="692" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A692" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B692" t="s">
+        <v>132</v>
+      </c>
+      <c r="C692" t="s">
+        <v>19</v>
+      </c>
+      <c r="D692">
+        <v>2</v>
+      </c>
+      <c r="E692" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="693" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A693" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B693" t="s">
+        <v>133</v>
+      </c>
+      <c r="C693" t="s">
+        <v>5</v>
+      </c>
+      <c r="D693">
+        <v>2</v>
+      </c>
+      <c r="E693" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="694" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A694" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B694" t="s">
+        <v>134</v>
+      </c>
+      <c r="C694" t="s">
+        <v>5</v>
+      </c>
+      <c r="D694">
+        <v>5</v>
+      </c>
+      <c r="E694" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="695" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A695" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B695" t="s">
+        <v>136</v>
+      </c>
+      <c r="C695" t="s">
+        <v>14</v>
+      </c>
+      <c r="D695">
+        <v>2</v>
+      </c>
+      <c r="E695" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="696" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A696" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B696" t="s">
+        <v>139</v>
+      </c>
+      <c r="C696" t="s">
+        <v>51</v>
+      </c>
+      <c r="D696">
+        <v>5</v>
+      </c>
+      <c r="E696" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="697" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A697" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B697" t="s">
+        <v>140</v>
+      </c>
+      <c r="C697" t="s">
+        <v>27</v>
+      </c>
+      <c r="D697">
+        <v>1</v>
+      </c>
+      <c r="E697" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="698" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A698" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B698" t="s">
+        <v>141</v>
+      </c>
+      <c r="C698" t="s">
+        <v>27</v>
+      </c>
+      <c r="D698">
+        <v>2</v>
+      </c>
+      <c r="E698" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="699" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A699" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B699" t="s">
+        <v>142</v>
+      </c>
+      <c r="C699" t="s">
+        <v>14</v>
+      </c>
+      <c r="D699">
+        <v>2</v>
+      </c>
+      <c r="E699" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="700" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A700" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B700" t="s">
+        <v>143</v>
+      </c>
+      <c r="C700" t="s">
+        <v>5</v>
+      </c>
+      <c r="D700">
+        <v>1</v>
+      </c>
+      <c r="E700" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="701" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A701" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B701" t="s">
+        <v>144</v>
+      </c>
+      <c r="C701" t="s">
+        <v>9</v>
+      </c>
+      <c r="D701">
+        <v>2</v>
+      </c>
+      <c r="E701" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="702" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A702" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B702" t="s">
+        <v>145</v>
+      </c>
+      <c r="C702" t="s">
+        <v>5</v>
+      </c>
+      <c r="D702">
+        <v>4</v>
+      </c>
+      <c r="E702" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="703" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A703" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B703" t="s">
+        <v>146</v>
+      </c>
+      <c r="C703" t="s">
+        <v>5</v>
+      </c>
+      <c r="D703">
+        <v>5</v>
+      </c>
+      <c r="E703" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="704" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A704" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B704" t="s">
+        <v>147</v>
+      </c>
+      <c r="C704" t="s">
+        <v>9</v>
+      </c>
+      <c r="D704">
+        <v>5</v>
+      </c>
+      <c r="E704" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="705" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A705" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B705" t="s">
+        <v>148</v>
+      </c>
+      <c r="C705" t="s">
+        <v>5</v>
+      </c>
+      <c r="D705">
+        <v>2</v>
+      </c>
+      <c r="E705" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="706" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A706" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B706" t="s">
+        <v>149</v>
+      </c>
+      <c r="C706" t="s">
+        <v>5</v>
+      </c>
+      <c r="D706">
+        <v>1</v>
+      </c>
+      <c r="E706" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="707" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A707" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B707" t="s">
+        <v>150</v>
+      </c>
+      <c r="C707" t="s">
+        <v>27</v>
+      </c>
+      <c r="D707">
+        <v>5</v>
+      </c>
+      <c r="E707" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="708" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A708" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B708" t="s">
+        <v>152</v>
+      </c>
+      <c r="C708" t="s">
+        <v>14</v>
+      </c>
+      <c r="D708">
+        <v>2</v>
+      </c>
+      <c r="E708" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="709" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A709" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B709" t="s">
+        <v>154</v>
+      </c>
+      <c r="C709" t="s">
+        <v>9</v>
+      </c>
+      <c r="D709">
+        <v>2</v>
+      </c>
+      <c r="E709" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="710" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A710" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B710" t="s">
+        <v>156</v>
+      </c>
+      <c r="C710" t="s">
+        <v>14</v>
+      </c>
+      <c r="D710">
+        <v>2</v>
+      </c>
+      <c r="E710" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="711" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A711" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B711" t="s">
+        <v>157</v>
+      </c>
+      <c r="C711" t="s">
+        <v>14</v>
+      </c>
+      <c r="D711">
+        <v>2</v>
+      </c>
+      <c r="E711" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="712" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A712" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B712" t="s">
+        <v>158</v>
+      </c>
+      <c r="C712" t="s">
+        <v>9</v>
+      </c>
+      <c r="D712">
+        <v>2</v>
+      </c>
+      <c r="E712" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="713" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A713" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B713" t="s">
+        <v>159</v>
+      </c>
+      <c r="C713" t="s">
+        <v>24</v>
+      </c>
+      <c r="D713">
+        <v>5</v>
+      </c>
+      <c r="E713" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="714" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A714" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B714" t="s">
+        <v>160</v>
+      </c>
+      <c r="C714" t="s">
+        <v>14</v>
+      </c>
+      <c r="D714">
+        <v>4</v>
+      </c>
+      <c r="E714" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="715" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A715" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B715" t="s">
+        <v>485</v>
+      </c>
+      <c r="C715" t="s">
+        <v>62</v>
+      </c>
+      <c r="D715">
+        <v>4</v>
+      </c>
+      <c r="E715" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="716" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A716" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B716" t="s">
+        <v>161</v>
+      </c>
+      <c r="C716" t="s">
+        <v>14</v>
+      </c>
+      <c r="D716">
+        <v>2</v>
+      </c>
+      <c r="E716" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="717" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A717" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B717" t="s">
+        <v>164</v>
+      </c>
+      <c r="C717" t="s">
+        <v>24</v>
+      </c>
+      <c r="D717">
+        <v>5</v>
+      </c>
+      <c r="E717" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="718" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A718" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B718" t="s">
+        <v>165</v>
+      </c>
+      <c r="C718" t="s">
+        <v>5</v>
+      </c>
+      <c r="D718">
+        <v>3</v>
+      </c>
+      <c r="E718" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="719" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A719" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B719" t="s">
+        <v>166</v>
+      </c>
+      <c r="C719" t="s">
+        <v>19</v>
+      </c>
+      <c r="D719">
+        <v>2</v>
+      </c>
+      <c r="E719" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="720" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A720" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B720" t="s">
+        <v>168</v>
+      </c>
+      <c r="C720" t="s">
+        <v>5</v>
+      </c>
+      <c r="D720">
+        <v>5</v>
+      </c>
+      <c r="E720" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="721" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A721" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B721" t="s">
+        <v>169</v>
+      </c>
+      <c r="C721" t="s">
+        <v>19</v>
+      </c>
+      <c r="D721">
+        <v>2</v>
+      </c>
+      <c r="E721" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="722" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A722" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B722" t="s">
+        <v>170</v>
+      </c>
+      <c r="C722" t="s">
+        <v>14</v>
+      </c>
+      <c r="D722">
+        <v>2</v>
+      </c>
+      <c r="E722" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="723" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A723" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B723" t="s">
+        <v>171</v>
+      </c>
+      <c r="C723" t="s">
+        <v>24</v>
+      </c>
+      <c r="D723">
+        <v>4</v>
+      </c>
+      <c r="E723" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="724" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A724" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B724" t="s">
+        <v>173</v>
+      </c>
+      <c r="C724" t="s">
+        <v>14</v>
+      </c>
+      <c r="D724">
+        <v>1</v>
+      </c>
+      <c r="E724" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="725" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A725" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B725" t="s">
+        <v>174</v>
+      </c>
+      <c r="C725" t="s">
+        <v>19</v>
+      </c>
+      <c r="D725">
+        <v>4</v>
+      </c>
+      <c r="E725" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="726" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A726" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B726" t="s">
+        <v>176</v>
+      </c>
+      <c r="C726" t="s">
+        <v>9</v>
+      </c>
+      <c r="D726">
+        <v>5</v>
+      </c>
+      <c r="E726" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="727" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A727" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B727" t="s">
+        <v>178</v>
+      </c>
+      <c r="C727" t="s">
+        <v>27</v>
+      </c>
+      <c r="D727">
+        <v>1</v>
+      </c>
+      <c r="E727" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="728" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A728" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B728" t="s">
+        <v>179</v>
+      </c>
+      <c r="C728" t="s">
+        <v>14</v>
+      </c>
+      <c r="D728">
+        <v>5</v>
+      </c>
+      <c r="E728" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="729" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A729" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B729" t="s">
+        <v>181</v>
+      </c>
+      <c r="C729" t="s">
+        <v>14</v>
+      </c>
+      <c r="D729">
+        <v>3</v>
+      </c>
+      <c r="E729" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="730" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A730" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B730" t="s">
+        <v>182</v>
+      </c>
+      <c r="C730" t="s">
+        <v>27</v>
+      </c>
+      <c r="D730">
+        <v>5</v>
+      </c>
+      <c r="E730" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="731" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A731" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B731" t="s">
+        <v>184</v>
+      </c>
+      <c r="C731" t="s">
+        <v>24</v>
+      </c>
+      <c r="D731">
+        <v>4</v>
+      </c>
+      <c r="E731" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="732" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A732" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B732" t="s">
+        <v>186</v>
+      </c>
+      <c r="C732" t="s">
+        <v>9</v>
+      </c>
+      <c r="D732">
+        <v>1</v>
+      </c>
+      <c r="E732" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="733" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A733" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B733" t="s">
+        <v>187</v>
+      </c>
+      <c r="C733" t="s">
+        <v>14</v>
+      </c>
+      <c r="D733">
+        <v>5</v>
+      </c>
+      <c r="E733" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="734" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A734" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B734" t="s">
+        <v>189</v>
+      </c>
+      <c r="C734" t="s">
+        <v>5</v>
+      </c>
+      <c r="D734">
+        <v>5</v>
+      </c>
+      <c r="E734" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="735" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A735" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B735" t="s">
+        <v>191</v>
+      </c>
+      <c r="C735" t="s">
+        <v>62</v>
+      </c>
+      <c r="D735">
+        <v>3</v>
+      </c>
+      <c r="E735" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="736" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A736" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B736" t="s">
+        <v>493</v>
+      </c>
+      <c r="C736" t="s">
+        <v>51</v>
+      </c>
+      <c r="D736">
+        <v>3</v>
+      </c>
+      <c r="E736" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="737" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A737" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B737" t="s">
+        <v>192</v>
+      </c>
+      <c r="C737" t="s">
+        <v>27</v>
+      </c>
+      <c r="D737">
+        <v>5</v>
+      </c>
+      <c r="E737" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="738" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A738" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B738" t="s">
+        <v>194</v>
+      </c>
+      <c r="C738" t="s">
+        <v>5</v>
+      </c>
+      <c r="D738">
+        <v>2</v>
+      </c>
+      <c r="E738" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="739" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A739" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B739" t="s">
+        <v>195</v>
+      </c>
+      <c r="C739" t="s">
+        <v>24</v>
+      </c>
+      <c r="D739">
+        <v>2</v>
+      </c>
+      <c r="E739" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="740" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A740" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B740" t="s">
+        <v>196</v>
+      </c>
+      <c r="C740" t="s">
+        <v>9</v>
+      </c>
+      <c r="D740">
+        <v>2</v>
+      </c>
+      <c r="E740" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="741" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A741" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B741" t="s">
+        <v>197</v>
+      </c>
+      <c r="C741" t="s">
+        <v>5</v>
+      </c>
+      <c r="D741">
+        <v>5</v>
+      </c>
+      <c r="E741" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="742" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A742" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B742" t="s">
+        <v>198</v>
+      </c>
+      <c r="C742" t="s">
+        <v>14</v>
+      </c>
+      <c r="D742">
+        <v>1</v>
+      </c>
+      <c r="E742" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="743" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A743" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B743" t="s">
+        <v>201</v>
+      </c>
+      <c r="C743" t="s">
+        <v>24</v>
+      </c>
+      <c r="D743">
+        <v>5</v>
+      </c>
+      <c r="E743" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="744" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A744" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B744" t="s">
+        <v>202</v>
+      </c>
+      <c r="C744" t="s">
+        <v>24</v>
+      </c>
+      <c r="D744">
+        <v>5</v>
+      </c>
+      <c r="E744" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="745" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A745" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B745" t="s">
+        <v>204</v>
+      </c>
+      <c r="C745" t="s">
+        <v>51</v>
+      </c>
+      <c r="D745">
+        <v>5</v>
+      </c>
+      <c r="E745" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="746" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A746" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B746" t="s">
+        <v>205</v>
+      </c>
+      <c r="C746" t="s">
+        <v>24</v>
+      </c>
+      <c r="D746">
+        <v>1</v>
+      </c>
+      <c r="E746" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="747" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A747" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B747" t="s">
+        <v>207</v>
+      </c>
+      <c r="C747" t="s">
+        <v>14</v>
+      </c>
+      <c r="D747">
+        <v>3</v>
+      </c>
+      <c r="E747" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="748" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A748" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B748" t="s">
+        <v>209</v>
+      </c>
+      <c r="C748" t="s">
+        <v>14</v>
+      </c>
+      <c r="D748">
+        <v>2</v>
+      </c>
+      <c r="E748" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="749" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A749" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B749" t="s">
+        <v>211</v>
+      </c>
+      <c r="C749" t="s">
+        <v>27</v>
+      </c>
+      <c r="D749">
+        <v>2</v>
+      </c>
+      <c r="E749" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="750" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A750" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B750" t="s">
+        <v>212</v>
+      </c>
+      <c r="C750" t="s">
+        <v>9</v>
+      </c>
+      <c r="D750">
+        <v>1</v>
+      </c>
+      <c r="E750" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="751" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A751" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B751" t="s">
+        <v>213</v>
+      </c>
+      <c r="C751" t="s">
+        <v>5</v>
+      </c>
+      <c r="D751">
+        <v>4</v>
+      </c>
+      <c r="E751" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="752" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A752" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B752" t="s">
+        <v>215</v>
+      </c>
+      <c r="C752" t="s">
+        <v>24</v>
+      </c>
+      <c r="D752">
+        <v>4</v>
+      </c>
+      <c r="E752" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="753" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A753" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B753" t="s">
+        <v>216</v>
+      </c>
+      <c r="C753" t="s">
+        <v>24</v>
+      </c>
+      <c r="D753">
+        <v>3</v>
+      </c>
+      <c r="E753" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="754" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A754" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B754" t="s">
+        <v>218</v>
+      </c>
+      <c r="C754" t="s">
+        <v>5</v>
+      </c>
+      <c r="D754">
+        <v>5</v>
+      </c>
+      <c r="E754" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="755" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A755" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B755" t="s">
+        <v>220</v>
+      </c>
+      <c r="C755" t="s">
+        <v>24</v>
+      </c>
+      <c r="D755">
+        <v>2</v>
+      </c>
+      <c r="E755" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="756" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A756" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B756" t="s">
+        <v>222</v>
+      </c>
+      <c r="C756" t="s">
+        <v>24</v>
+      </c>
+      <c r="D756">
+        <v>2</v>
+      </c>
+      <c r="E756" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="757" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A757" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B757" t="s">
+        <v>223</v>
+      </c>
+      <c r="C757" t="s">
+        <v>27</v>
+      </c>
+      <c r="D757">
+        <v>2</v>
+      </c>
+      <c r="E757" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="758" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A758" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B758" t="s">
+        <v>224</v>
+      </c>
+      <c r="C758" t="s">
+        <v>5</v>
+      </c>
+      <c r="D758">
+        <v>2</v>
+      </c>
+      <c r="E758" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="759" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A759" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B759" t="s">
+        <v>225</v>
+      </c>
+      <c r="C759" t="s">
+        <v>9</v>
+      </c>
+      <c r="D759">
+        <v>2</v>
+      </c>
+      <c r="E759" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="760" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A760" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B760" t="s">
+        <v>226</v>
+      </c>
+      <c r="C760" t="s">
+        <v>9</v>
+      </c>
+      <c r="D760">
+        <v>2</v>
+      </c>
+      <c r="E760" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="761" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A761" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B761" t="s">
+        <v>227</v>
+      </c>
+      <c r="C761" t="s">
+        <v>5</v>
+      </c>
+      <c r="D761">
+        <v>5</v>
+      </c>
+      <c r="E761" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="762" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A762" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B762" t="s">
+        <v>229</v>
+      </c>
+      <c r="C762" t="s">
+        <v>9</v>
+      </c>
+      <c r="D762">
+        <v>4</v>
+      </c>
+      <c r="E762" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="763" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A763" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B763" t="s">
+        <v>231</v>
+      </c>
+      <c r="C763" t="s">
+        <v>24</v>
+      </c>
+      <c r="D763">
+        <v>5</v>
+      </c>
+      <c r="E763" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="764" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A764" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B764" t="s">
+        <v>233</v>
+      </c>
+      <c r="C764" t="s">
+        <v>5</v>
+      </c>
+      <c r="D764">
+        <v>2</v>
+      </c>
+      <c r="E764" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="765" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A765" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B765" t="s">
+        <v>234</v>
+      </c>
+      <c r="C765" t="s">
+        <v>5</v>
+      </c>
+      <c r="D765">
+        <v>2</v>
+      </c>
+      <c r="E765" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="766" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A766" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B766" t="s">
+        <v>235</v>
+      </c>
+      <c r="C766" t="s">
+        <v>9</v>
+      </c>
+      <c r="D766">
+        <v>1</v>
+      </c>
+      <c r="E766" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="767" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A767" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B767" t="s">
+        <v>236</v>
+      </c>
+      <c r="C767" t="s">
+        <v>14</v>
+      </c>
+      <c r="D767">
+        <v>2</v>
+      </c>
+      <c r="E767" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="768" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A768" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B768" t="s">
+        <v>237</v>
+      </c>
+      <c r="C768" t="s">
+        <v>62</v>
+      </c>
+      <c r="D768">
+        <v>5</v>
+      </c>
+      <c r="E768" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="769" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A769" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B769" t="s">
+        <v>238</v>
+      </c>
+      <c r="C769" t="s">
+        <v>14</v>
+      </c>
+      <c r="D769">
+        <v>2</v>
+      </c>
+      <c r="E769" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="770" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A770" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B770" t="s">
+        <v>239</v>
+      </c>
+      <c r="C770" t="s">
+        <v>9</v>
+      </c>
+      <c r="D770">
+        <v>5</v>
+      </c>
+      <c r="E770" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="771" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A771" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B771" t="s">
+        <v>240</v>
+      </c>
+      <c r="C771" t="s">
+        <v>14</v>
+      </c>
+      <c r="D771">
+        <v>2</v>
+      </c>
+      <c r="E771" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="772" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A772" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B772" t="s">
+        <v>242</v>
+      </c>
+      <c r="C772" t="s">
+        <v>24</v>
+      </c>
+      <c r="D772">
+        <v>4</v>
+      </c>
+      <c r="E772" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="773" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A773" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B773" t="s">
+        <v>244</v>
+      </c>
+      <c r="C773" t="s">
+        <v>9</v>
+      </c>
+      <c r="D773">
+        <v>4</v>
+      </c>
+      <c r="E773" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="774" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A774" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B774" t="s">
+        <v>245</v>
+      </c>
+      <c r="C774" t="s">
+        <v>5</v>
+      </c>
+      <c r="D774">
+        <v>2</v>
+      </c>
+      <c r="E774" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="775" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A775" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B775" t="s">
+        <v>247</v>
+      </c>
+      <c r="C775" t="s">
+        <v>5</v>
+      </c>
+      <c r="D775">
+        <v>5</v>
+      </c>
+      <c r="E775" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="776" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A776" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B776" t="s">
+        <v>248</v>
+      </c>
+      <c r="C776" t="s">
+        <v>27</v>
+      </c>
+      <c r="D776">
+        <v>5</v>
+      </c>
+      <c r="E776" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="777" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A777" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B777" t="s">
+        <v>250</v>
+      </c>
+      <c r="C777" t="s">
+        <v>24</v>
+      </c>
+      <c r="D777">
+        <v>5</v>
+      </c>
+      <c r="E777" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="778" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A778" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B778" t="s">
+        <v>252</v>
+      </c>
+      <c r="C778" t="s">
+        <v>9</v>
+      </c>
+      <c r="D778">
+        <v>1</v>
+      </c>
+      <c r="E778" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="779" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A779" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B779" t="s">
+        <v>253</v>
+      </c>
+      <c r="C779" t="s">
+        <v>24</v>
+      </c>
+      <c r="D779">
+        <v>5</v>
+      </c>
+      <c r="E779" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="780" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A780" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B780" t="s">
+        <v>255</v>
+      </c>
+      <c r="C780" t="s">
+        <v>9</v>
+      </c>
+      <c r="D780">
+        <v>3</v>
+      </c>
+      <c r="E780" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="781" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A781" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B781" t="s">
+        <v>257</v>
+      </c>
+      <c r="C781" t="s">
+        <v>14</v>
+      </c>
+      <c r="D781">
+        <v>3</v>
+      </c>
+      <c r="E781" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="782" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A782" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B782" t="s">
+        <v>258</v>
+      </c>
+      <c r="C782" t="s">
+        <v>14</v>
+      </c>
+      <c r="D782">
+        <v>4</v>
+      </c>
+      <c r="E782" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="783" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A783" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B783" t="s">
+        <v>260</v>
+      </c>
+      <c r="C783" t="s">
+        <v>9</v>
+      </c>
+      <c r="D783">
+        <v>2</v>
+      </c>
+      <c r="E783" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="784" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A784" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B784" t="s">
+        <v>261</v>
+      </c>
+      <c r="C784" t="s">
+        <v>5</v>
+      </c>
+      <c r="D784">
+        <v>3</v>
+      </c>
+      <c r="E784" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="785" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A785" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B785" t="s">
+        <v>262</v>
+      </c>
+      <c r="C785" t="s">
+        <v>24</v>
+      </c>
+      <c r="D785">
+        <v>5</v>
+      </c>
+      <c r="E785" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="786" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A786" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B786" t="s">
+        <v>263</v>
+      </c>
+      <c r="C786" t="s">
+        <v>24</v>
+      </c>
+      <c r="D786">
+        <v>5</v>
+      </c>
+      <c r="E786" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="787" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A787" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B787" t="s">
+        <v>264</v>
+      </c>
+      <c r="C787" t="s">
+        <v>9</v>
+      </c>
+      <c r="D787">
+        <v>2</v>
+      </c>
+      <c r="E787" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="788" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A788" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B788" t="s">
+        <v>265</v>
+      </c>
+      <c r="C788" t="s">
+        <v>9</v>
+      </c>
+      <c r="D788">
+        <v>5</v>
+      </c>
+      <c r="E788" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="789" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A789" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B789" t="s">
+        <v>267</v>
+      </c>
+      <c r="C789" t="s">
+        <v>24</v>
+      </c>
+      <c r="D789">
+        <v>5</v>
+      </c>
+      <c r="E789" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="790" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A790" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B790" t="s">
+        <v>269</v>
+      </c>
+      <c r="C790" t="s">
+        <v>5</v>
+      </c>
+      <c r="D790">
+        <v>2</v>
+      </c>
+      <c r="E790" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="791" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A791" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B791" t="s">
+        <v>270</v>
+      </c>
+      <c r="C791" t="s">
+        <v>14</v>
+      </c>
+      <c r="D791">
+        <v>3</v>
+      </c>
+      <c r="E791" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="792" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A792" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B792" t="s">
+        <v>271</v>
+      </c>
+      <c r="C792" t="s">
+        <v>5</v>
+      </c>
+      <c r="D792">
+        <v>3</v>
+      </c>
+      <c r="E792" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="793" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A793" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B793" t="s">
+        <v>272</v>
+      </c>
+      <c r="C793" t="s">
+        <v>9</v>
+      </c>
+      <c r="D793">
+        <v>3</v>
+      </c>
+      <c r="E793" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="794" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A794" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B794" t="s">
+        <v>273</v>
+      </c>
+      <c r="C794" t="s">
+        <v>19</v>
+      </c>
+      <c r="D794">
+        <v>5</v>
+      </c>
+      <c r="E794" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="795" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A795" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B795" t="s">
+        <v>274</v>
+      </c>
+      <c r="C795" t="s">
+        <v>9</v>
+      </c>
+      <c r="D795">
+        <v>4</v>
+      </c>
+      <c r="E795" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="796" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A796" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B796" t="s">
+        <v>275</v>
+      </c>
+      <c r="C796" t="s">
+        <v>24</v>
+      </c>
+      <c r="D796">
+        <v>2</v>
+      </c>
+      <c r="E796" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="797" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A797" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B797" t="s">
+        <v>276</v>
+      </c>
+      <c r="C797" t="s">
+        <v>9</v>
+      </c>
+      <c r="D797">
+        <v>5</v>
+      </c>
+      <c r="E797" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="798" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A798" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B798" t="s">
+        <v>277</v>
+      </c>
+      <c r="C798" t="s">
+        <v>24</v>
+      </c>
+      <c r="D798">
+        <v>2</v>
+      </c>
+      <c r="E798" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="799" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A799" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B799" t="s">
+        <v>278</v>
+      </c>
+      <c r="C799" t="s">
+        <v>14</v>
+      </c>
+      <c r="D799">
+        <v>5</v>
+      </c>
+      <c r="E799" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="800" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A800" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B800" t="s">
+        <v>279</v>
+      </c>
+      <c r="C800" t="s">
+        <v>5</v>
+      </c>
+      <c r="D800">
+        <v>3</v>
+      </c>
+      <c r="E800" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="801" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A801" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B801" t="s">
+        <v>280</v>
+      </c>
+      <c r="C801" t="s">
+        <v>9</v>
+      </c>
+      <c r="D801">
+        <v>4</v>
+      </c>
+      <c r="E801" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="802" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A802" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B802" t="s">
+        <v>512</v>
+      </c>
+      <c r="C802" t="s">
+        <v>51</v>
+      </c>
+      <c r="D802">
+        <v>3</v>
+      </c>
+      <c r="E802" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="803" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A803" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B803" t="s">
+        <v>281</v>
+      </c>
+      <c r="C803" t="s">
+        <v>24</v>
+      </c>
+      <c r="D803">
+        <v>5</v>
+      </c>
+      <c r="E803" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="804" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A804" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B804" t="s">
+        <v>282</v>
+      </c>
+      <c r="C804" t="s">
+        <v>9</v>
+      </c>
+      <c r="D804">
+        <v>2</v>
+      </c>
+      <c r="E804" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="805" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A805" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B805" t="s">
+        <v>283</v>
+      </c>
+      <c r="C805" t="s">
+        <v>5</v>
+      </c>
+      <c r="D805">
+        <v>2</v>
+      </c>
+      <c r="E805" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="806" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A806" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B806" t="s">
+        <v>284</v>
+      </c>
+      <c r="C806" t="s">
+        <v>24</v>
+      </c>
+      <c r="D806">
+        <v>3</v>
+      </c>
+      <c r="E806" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="807" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A807" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B807" t="s">
+        <v>285</v>
+      </c>
+      <c r="C807" t="s">
+        <v>9</v>
+      </c>
+      <c r="D807">
+        <v>4</v>
+      </c>
+      <c r="E807" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="808" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A808" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B808" t="s">
+        <v>286</v>
+      </c>
+      <c r="C808" t="s">
+        <v>9</v>
+      </c>
+      <c r="D808">
+        <v>5</v>
+      </c>
+      <c r="E808" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="809" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A809" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B809" t="s">
+        <v>287</v>
+      </c>
+      <c r="C809" t="s">
+        <v>24</v>
+      </c>
+      <c r="D809">
+        <v>2</v>
+      </c>
+      <c r="E809" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="810" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A810" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B810" t="s">
+        <v>288</v>
+      </c>
+      <c r="C810" t="s">
+        <v>14</v>
+      </c>
+      <c r="D810">
+        <v>2</v>
+      </c>
+      <c r="E810" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="811" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A811" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B811" t="s">
+        <v>289</v>
+      </c>
+      <c r="C811" t="s">
+        <v>27</v>
+      </c>
+      <c r="D811">
+        <v>2</v>
+      </c>
+      <c r="E811" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="812" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A812" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B812" t="s">
+        <v>290</v>
+      </c>
+      <c r="C812" t="s">
+        <v>9</v>
+      </c>
+      <c r="D812">
+        <v>5</v>
+      </c>
+      <c r="E812" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="813" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A813" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B813" t="s">
+        <v>292</v>
+      </c>
+      <c r="C813" t="s">
+        <v>5</v>
+      </c>
+      <c r="D813">
+        <v>4</v>
+      </c>
+      <c r="E813" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="814" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A814" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B814" t="s">
+        <v>294</v>
+      </c>
+      <c r="C814" t="s">
+        <v>5</v>
+      </c>
+      <c r="D814">
+        <v>4</v>
+      </c>
+      <c r="E814" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="815" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A815" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B815" t="s">
+        <v>295</v>
+      </c>
+      <c r="C815" t="s">
+        <v>14</v>
+      </c>
+      <c r="D815">
+        <v>3</v>
+      </c>
+      <c r="E815" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="816" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A816" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B816" t="s">
+        <v>297</v>
+      </c>
+      <c r="C816" t="s">
+        <v>24</v>
+      </c>
+      <c r="D816">
+        <v>2</v>
+      </c>
+      <c r="E816" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="817" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A817" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B817" t="s">
+        <v>298</v>
+      </c>
+      <c r="C817" t="s">
+        <v>14</v>
+      </c>
+      <c r="D817">
+        <v>4</v>
+      </c>
+      <c r="E817" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="818" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A818" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B818" t="s">
+        <v>299</v>
+      </c>
+      <c r="C818" t="s">
+        <v>5</v>
+      </c>
+      <c r="D818">
+        <v>2</v>
+      </c>
+      <c r="E818" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="819" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A819" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B819" t="s">
+        <v>300</v>
+      </c>
+      <c r="C819" t="s">
+        <v>9</v>
+      </c>
+      <c r="D819">
+        <v>5</v>
+      </c>
+      <c r="E819" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="820" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A820" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B820" t="s">
+        <v>301</v>
+      </c>
+      <c r="C820" t="s">
+        <v>9</v>
+      </c>
+      <c r="D820">
+        <v>3</v>
+      </c>
+      <c r="E820" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="821" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A821" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B821" t="s">
+        <v>302</v>
+      </c>
+      <c r="C821" t="s">
+        <v>9</v>
+      </c>
+      <c r="D821">
+        <v>5</v>
+      </c>
+      <c r="E821" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="822" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A822" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B822" t="s">
+        <v>304</v>
+      </c>
+      <c r="C822" t="s">
+        <v>24</v>
+      </c>
+      <c r="D822">
+        <v>5</v>
+      </c>
+      <c r="E822" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="823" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A823" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B823" t="s">
+        <v>521</v>
+      </c>
+      <c r="C823" t="s">
+        <v>62</v>
+      </c>
+      <c r="D823">
+        <v>1</v>
+      </c>
+      <c r="E823" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="824" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A824" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B824" t="s">
+        <v>306</v>
+      </c>
+      <c r="C824" t="s">
+        <v>27</v>
+      </c>
+      <c r="D824">
+        <v>1</v>
+      </c>
+      <c r="E824" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="825" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A825" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B825" t="s">
+        <v>308</v>
+      </c>
+      <c r="C825" t="s">
+        <v>14</v>
+      </c>
+      <c r="D825">
+        <v>5</v>
+      </c>
+      <c r="E825" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="826" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A826" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B826" t="s">
+        <v>310</v>
+      </c>
+      <c r="C826" t="s">
+        <v>14</v>
+      </c>
+      <c r="D826">
+        <v>1</v>
+      </c>
+      <c r="E826" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="827" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A827" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B827" t="s">
+        <v>311</v>
+      </c>
+      <c r="C827" t="s">
+        <v>5</v>
+      </c>
+      <c r="D827">
+        <v>4</v>
+      </c>
+      <c r="E827" t="s">
+        <v>523</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Initial commit: dashboard code with KPI tab fixes6
</commit_message>
<xml_diff>
--- a/Tutor_Concerns.xlsx
+++ b/Tutor_Concerns.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tyler_harrington2/Desktop/FL_Dashboards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E0E97A2B-DF18-0041-8DDB-914C22B5E137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{5B3D2AC9-73B2-0841-A9CC-D68F5A87B440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14860" xr2:uid="{92DEE1D6-509C-344A-AA8F-D8DD2317BD81}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{92DEE1D6-509C-344A-AA8F-D8DD2317BD81}"/>
   </bookViews>
   <sheets>
     <sheet name="Concerns" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="3309" uniqueCount="525">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="4137" uniqueCount="602">
   <si>
     <t>Tutor Name</t>
   </si>
@@ -1611,6 +1611,237 @@
   </si>
   <si>
     <t>11/2/25 - 11/30/25</t>
+  </si>
+  <si>
+    <t>Ratio of PPW Events with Attached PPW &lt; 1/2; % of Active Students with Progress Updates Completed in last 2 months &lt; 70%; Diff M2M % of Active Students with Progress Updates Completed in last 2 months &lt; -20%; Prep Time % &gt; 15%; Diff M2M % to Delivery Target &lt; -20% and % to Delivery Target &lt; 85%</t>
+  </si>
+  <si>
+    <t>% Parent Updates &lt; 85%; % of Active Students with Progress Updates Completed in last 2 months &lt; 70%; Prep Time % &gt; 15%; Diff M2M Prep Time % &gt; 10%; Diff M2M % to Availability Target &lt; -10% and % to Availability Target &lt; 95%</t>
+  </si>
+  <si>
+    <t>% Parent Updates &lt; 85%; % Sessions on Time &lt; 85%</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; Ratio of PPW Events with Attached PPW &lt; 1/2; Diff M2M % to Delivery Target &lt; -20% and % to Delivery Target &lt; 85%; Diff M2M % to Availability Target &lt; -10% and % to Availability Target &lt; 95%; Bottom 10% in % to Delivery Target for tier</t>
+  </si>
+  <si>
+    <t>Amy Kim</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; % Parent Updates &lt; 85%; Diff M2M % to Delivery Target &lt; -20% and % to Delivery Target &lt; 85%; Diff M2M % to Availability Target &lt; -10% and % to Availability Target &lt; 95%; Bottom 10% in % to Delivery Target for tier</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; Ratio of PPW Events with Attached PPW &lt; 1/2; % of Active Students with Progress Updates Completed in last 2 months &lt; 50%; Prep Time % &gt; 15%; Diff M2M % to Delivery Target &lt; -20% and % to Delivery Target &lt; 85%; Diff M2M % to Availability Target &lt; -10% and % to Availability Target &lt; 95%</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; Ratio of PPW Events with Attached PPW &lt; 1/2</t>
+  </si>
+  <si>
+    <t>Diff M2M Prep Time % &gt; 10%; Diff M2M % to Delivery Target &lt; -20% and % to Delivery Target &lt; 85%</t>
+  </si>
+  <si>
+    <t>Autumn Reed</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; Ratio of PPW Events with Attached PPW &lt; 1/2; Bottom 10% in % to Delivery Target for tier</t>
+  </si>
+  <si>
+    <t>% Sessions on Time &lt; 85%; % of Active Students with Progress Updates Completed in last 2 months &lt; 70%; Prep Time % &gt; 15%</t>
+  </si>
+  <si>
+    <t>Prep Time % &gt; 15%; Diff M2M % to Availability Target &lt; -10% and % to Availability Target &lt; 95%</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; % of Active Students with Progress Updates Completed in last 2 months &lt; 50%; Prep Time % &gt; 15%; Diff M2M % to Delivery Target &lt; -20% and % to Delivery Target &lt; 85%; Diff M2M % to Availability Target &lt; -10% and % to Availability Target &lt; 95%; Bottom 10% in % to Delivery Target for tier</t>
+  </si>
+  <si>
+    <t>% Parent Updates &lt; 85%; % of Active Students with Progress Updates Completed in last 2 months &lt; 50%; Prep Time % &gt; 15%; Diff M2M Prep Time % &gt; 10%; Bottom 10% in % to Delivery Target for tier</t>
+  </si>
+  <si>
+    <t>Ratio of PPW Events with Attached PPW &lt; 1/2; Diff M2M % to Delivery Target &lt; -20% and % to Delivery Target &lt; 85%; Bottom 10% in % to Delivery Target for tier</t>
+  </si>
+  <si>
+    <t>Cheyanne Jones</t>
+  </si>
+  <si>
+    <t>% Parent Updates &lt; 85%; % Sessions on Time &lt; 85%; Ratio of PPW Events with Attached PPW &lt; 1/2; % of Active Students with Progress Updates Completed in last 2 months &lt; 50%; Prep Time % &gt; 15%; Diff M2M Prep Time % &gt; 10%</t>
+  </si>
+  <si>
+    <t>% Parent Updates &lt; 85%; % Sessions on Time &lt; 90%; Ratio of PPW Events with Attached PPW &lt; 1/2; % of Active Students with Progress Updates Completed in last 2 months &lt; 60%</t>
+  </si>
+  <si>
+    <t>Derek Fox</t>
+  </si>
+  <si>
+    <t>Ratio of PPW Events with Attached PPW &lt; 1/2; Bottom 10% in % to Delivery Target for tier</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; Ratio of PPW Events with Attached PPW &lt; 1/2; Prep Time % &gt; 15%; Diff M2M % to Delivery Target &lt; -20% and % to Delivery Target &lt; 85%; Diff M2M % to Availability Target &lt; -10% and % to Availability Target &lt; 95%</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; % Parent Updates &lt; 85%; % of Active Students with Progress Updates Completed in last 2 months &lt; 50%; Bottom 10% in % to Delivery Target for tier</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; Ratio of PPW Events with Attached PPW &lt; 1/2; Prep Time % &gt; 15%; Diff M2M Prep Time % &gt; 10%</t>
+  </si>
+  <si>
+    <t>Ratio of PPW Events with Attached PPW &lt; 1/2; % of Active Students with Progress Updates Completed in last 2 months &lt; 60%; Prep Time % &gt; 15%; Diff M2M % to Availability Target &lt; -10% and % to Availability Target &lt; 95%</t>
+  </si>
+  <si>
+    <t>Ratio of PPW Events with Attached PPW &lt; 1/2; % of Active Students with Progress Updates Completed in last 2 months &lt; 50%; Diff M2M % of Active Students with Progress Updates Completed in last 2 months &lt; -20%; Prep Time % &gt; 15%; Diff M2M % to Delivery Target &lt; -20% and % to Delivery Target &lt; 85%</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; % Sessions on Time &lt; 85%; Ratio of PPW Events with Attached PPW &lt; 1/2; Diff M2M % to Delivery Target &lt; -20% and % to Delivery Target &lt; 85%; Diff M2M % to Availability Target &lt; -10% and % to Availability Target &lt; 95%</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; Ratio of PPW Events with Attached PPW &lt; 1/2; % of Active Students with Progress Updates Completed in last 2 months &lt; 70%; Diff M2M % to Availability Target &lt; -10% and % to Availability Target &lt; 95%</t>
+  </si>
+  <si>
+    <t>Ratio of PPW Events with Attached PPW &lt; 1/2; % of Active Students with Progress Updates Completed in last 2 months &lt; 50%; Diff M2M % of Active Students with Progress Updates Completed in last 2 months &lt; -20%; Prep Time % &gt; 15%; Diff M2M Prep Time % &gt; 10%</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; Prep Time % &gt; 15%; Diff M2M % to Delivery Target &lt; -20% and % to Delivery Target &lt; 85%; Diff M2M % to Availability Target &lt; -10% and % to Availability Target &lt; 95%</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; % Parent Updates &lt; 85%; Ratio of PPW Events with Attached PPW &lt; 1/2; Prep Time % &gt; 15%</t>
+  </si>
+  <si>
+    <t>% Sessions on Time &lt; 90%; Ratio of PPW Events with Attached PPW &lt; 1/2; % of Active Students with Progress Updates Completed in last 2 months &lt; 50%; Diff M2M % of Active Students with Progress Updates Completed in last 2 months &lt; -20%; Prep Time % &gt; 15%</t>
+  </si>
+  <si>
+    <t>Jocelyne Nolasco</t>
+  </si>
+  <si>
+    <t>% Parent Updates &lt; 85%; % Sessions on Time &lt; 85%; % of Active Students with Progress Updates Completed in last 2 months &lt; 50%; Prep Time % &gt; 15%</t>
+  </si>
+  <si>
+    <t>Juan Nunez</t>
+  </si>
+  <si>
+    <t>Karleigh Arrington</t>
+  </si>
+  <si>
+    <t>% Parent Updates &lt; 85%; Prep Time % &gt; 15%; Diff M2M % to Availability Target &lt; -10% and % to Availability Target &lt; 95%</t>
+  </si>
+  <si>
+    <t>Ratio of PPW Events with Attached PPW &lt; 1/2; % of Active Students with Progress Updates Completed in last 2 months &lt; 60%; Prep Time % &gt; 15%; Diff M2M % to Delivery Target &lt; -20% and % to Delivery Target &lt; 85%</t>
+  </si>
+  <si>
+    <t>% Sessions on Time &lt; 90%; Prep Time % &gt; 15%; Avg. NPS Score &lt; 8</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; % Sessions on Time &lt; 85%; Ratio of PPW Events with Attached PPW &lt; 1/2; Prep Time % &gt; 15%; Diff M2M Prep Time % &gt; 10%</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; % Parent Updates &lt; 90%; Prep Time % &gt; 15%</t>
+  </si>
+  <si>
+    <t>Prep Time % &gt; 15%; Avg. NPS Score &lt; 8; Diff M2M % to Delivery Target &lt; -20% and % to Delivery Target &lt; 85%</t>
+  </si>
+  <si>
+    <t>% Parent Updates &lt; 90%; Ratio of PPW Events with Attached PPW &lt; 1/2; Prep Time % &gt; 15%; Diff M2M Prep Time % &gt; 10%; Diff M2M % to Delivery Target &lt; -20% and % to Delivery Target &lt; 85%</t>
+  </si>
+  <si>
+    <t>% Parent Updates &lt; 90%; Ratio of PPW Events with Attached PPW &lt; 1/2; Prep Time % &gt; 15%; Diff M2M Prep Time % &gt; 10%</t>
+  </si>
+  <si>
+    <t>% Parent Updates &lt; 85%; Ratio of PPW Events with Attached PPW &lt; 1/2; Prep Time % &gt; 15%; Diff M2M Prep Time % &gt; 10%</t>
+  </si>
+  <si>
+    <t>% Parent Updates &lt; 85%; Ratio of PPW Events with Attached PPW &lt; 1/2; Diff M2M % to Delivery Target &lt; -20% and % to Delivery Target &lt; 85%</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; Ratio of PPW Events with Attached PPW &lt; 1/2; Prep Time % &gt; 15%; Diff M2M Prep Time % &gt; 10%; Bottom 10% in % to Delivery Target for tier</t>
+  </si>
+  <si>
+    <t>Mauricio (Maui) Monroy</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; Ratio of PPW Events with Attached PPW &lt; 1/2; % of Active Students with Progress Updates Completed in last 2 months &lt; 50%; Prep Time % &gt; 15%; Diff M2M % to Availability Target &lt; -10% and % to Availability Target &lt; 95%</t>
+  </si>
+  <si>
+    <t>% Parent Updates &lt; 90%; Prep Time % &gt; 15%; Diff M2M % to Availability Target &lt; -10% and % to Availability Target &lt; 95%</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; % Parent Updates &lt; 85%; % of Active Students with Progress Updates Completed in last 2 months &lt; 70%; Prep Time % &gt; 15%; Diff M2M Prep Time % &gt; 10%; Diff M2M % to Delivery Target &lt; -20% and % to Delivery Target &lt; 85%; Diff M2M % to Availability Target &lt; -10% and % to Availability Target &lt; 95%</t>
+  </si>
+  <si>
+    <t>Ratio of PPW Events with Attached PPW &lt; 1/2; Prep Time % &gt; 15%; Diff M2M % to Delivery Target &lt; -20% and % to Delivery Target &lt; 85%; Bottom 10% in % to Delivery Target for tier</t>
+  </si>
+  <si>
+    <t>Natalie Angstadt</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; % Parent Updates &lt; 85%; Ratio of PPW Events with Attached PPW &lt; 1/2; Prep Time % &gt; 15%; Diff M2M % to Delivery Target &lt; -20% and % to Delivery Target &lt; 85%</t>
+  </si>
+  <si>
+    <t>% Parent Updates &lt; 85%; % of Active Students with Progress Updates Completed in last 2 months &lt; 70%; Prep Time % &gt; 15%</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; Ratio of PPW Events with Attached PPW &lt; 1/2; Prep Time % &gt; 15%</t>
+  </si>
+  <si>
+    <t>% Parent Updates &lt; 85%; % Sessions on Time &lt; 90%; Ratio of PPW Events with Attached PPW &lt; 1/2; Diff M2M % to Delivery Target &lt; -20% and % to Delivery Target &lt; 85%</t>
+  </si>
+  <si>
+    <t>% Parent Updates &lt; 85%; % Sessions on Time &lt; 85%; Ratio of PPW Events with Attached PPW &lt; 1/2; % of Active Students with Progress Updates Completed in last 2 months &lt; 70%; Diff M2M % to Delivery Target &lt; -20% and % to Delivery Target &lt; 85%</t>
+  </si>
+  <si>
+    <t>Ratio of PPW Events with Attached PPW &lt; 1/2; Diff M2M % to Delivery Target &lt; -20% and % to Delivery Target &lt; 85%; Diff M2M % to Availability Target &lt; -10% and % to Availability Target &lt; 95%</t>
+  </si>
+  <si>
+    <t>Ratio of PPW Events with Attached PPW &lt; 1/2; % of Active Students with Progress Updates Completed in last 2 months &lt; 60%; Diff M2M Prep Time % &gt; 10%</t>
+  </si>
+  <si>
+    <t>Rebekah Nachian</t>
+  </si>
+  <si>
+    <t>Prep Time % &gt; 15%; Diff M2M Prep Time % &gt; 10%; Avg. NPS Score &lt; 8</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; % of Active Students with Progress Updates Completed in last 2 months &lt; 70%; Prep Time % &gt; 15%</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; % Parent Updates &lt; 90%; Ratio of PPW Events with Attached PPW &lt; 1/2; % of Active Students with Progress Updates Completed in last 2 months &lt; 60%; Prep Time % &gt; 15%; Diff M2M Prep Time % &gt; 10%; Diff M2M % to Delivery Target &lt; -20% and % to Delivery Target &lt; 85%; Diff M2M % to Availability Target &lt; -10% and % to Availability Target &lt; 95%</t>
+  </si>
+  <si>
+    <t>% Sessions on Time &lt; 85%; Ratio of PPW Events with Attached PPW &lt; 1/2; Prep Time % &gt; 15%; Diff M2M Prep Time % &gt; 10%; Diff M2M % to Delivery Target &lt; -20% and % to Delivery Target &lt; 85%</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; Avg. NPS Score &lt; 8</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; Ratio of PPW Events with Attached PPW &lt; 1/2; % of Active Students with Progress Updates Completed in last 2 months &lt; 70%</t>
+  </si>
+  <si>
+    <t>% Sessions on Time &lt; 85%; % of Active Students with Progress Updates Completed in last 2 months &lt; 50%</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; % Parent Updates &lt; 85%; Ratio of PPW Events with Attached PPW &lt; 1/2; Diff M2M % of Active Students with Progress Updates Completed in last 2 months &lt; -20%; Prep Time % &gt; 15%; Bottom 10% in % to Delivery Target for tier</t>
+  </si>
+  <si>
+    <t>% of Active Students with Progress Updates Completed in last 2 months &lt; 50%; Diff M2M Prep Time % &gt; 10%</t>
+  </si>
+  <si>
+    <t>% Parent Updates &lt; 85%; Ratio of PPW Events with Attached PPW &lt; 1/2; % of Active Students with Progress Updates Completed in last 2 months &lt; 60%; Prep Time % &gt; 15%; Avg. NPS Score &lt; 8; Diff M2M % to Delivery Target &lt; -20% and % to Delivery Target &lt; 85%</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; % Parent Updates &lt; 85%; % of Active Students with Progress Updates Completed in last 2 months &lt; 60%; Diff M2M % to Delivery Target &lt; -20% and % to Delivery Target &lt; 85%; Diff M2M % to Availability Target &lt; -10% and % to Availability Target &lt; 95%</t>
+  </si>
+  <si>
+    <t>% Parent Updates &lt; 85%; % of Active Students with Progress Updates Completed in last 2 months &lt; 70%; Weighted Repurchases = 0</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; Prep Time % &gt; 15%; Diff M2M % to Delivery Target &lt; -20% and % to Delivery Target &lt; 85%</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; % Parent Updates &lt; 85%; Ratio of PPW Events with Attached PPW &lt; 1/2; Diff M2M % to Delivery Target &lt; -20% and % to Delivery Target &lt; 85%; Diff M2M % to Availability Target &lt; -10% and % to Availability Target &lt; 95%; Bottom 10% in % to Delivery Target for tier</t>
+  </si>
+  <si>
+    <t>% to Availability Target &lt; 90%; Ratio of PPW Events with Attached PPW &lt; 1/2; Diff M2M % to Delivery Target &lt; -20% and % to Delivery Target &lt; 85%; Diff M2M % to Availability Target &lt; -10% and % to Availability Target &lt; 95%</t>
+  </si>
+  <si>
+    <t>11/30/25 - 12/27/25</t>
   </si>
 </sst>
 </file>
@@ -2480,10 +2711,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDA4CB91-83C8-694D-BBCD-170E9881DA10}">
-  <dimension ref="A1:E827"/>
+  <dimension ref="A1:E1034"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A504" workbookViewId="0">
-      <selection activeCell="D614" sqref="D614"/>
+    <sheetView tabSelected="1" topLeftCell="A1007" workbookViewId="0">
+      <selection activeCell="D827" sqref="D827"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16550,6 +16781,3525 @@
         <v>523</v>
       </c>
     </row>
+    <row r="828" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A828" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B828" t="s">
+        <v>7</v>
+      </c>
+      <c r="C828" t="s">
+        <v>5</v>
+      </c>
+      <c r="D828">
+        <v>2</v>
+      </c>
+      <c r="E828" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="829" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A829" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B829" t="s">
+        <v>8</v>
+      </c>
+      <c r="C829" t="s">
+        <v>9</v>
+      </c>
+      <c r="D829">
+        <v>3</v>
+      </c>
+      <c r="E829" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="830" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A830" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B830" t="s">
+        <v>11</v>
+      </c>
+      <c r="C830" t="s">
+        <v>5</v>
+      </c>
+      <c r="D830">
+        <v>1</v>
+      </c>
+      <c r="E830" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="831" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A831" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B831" t="s">
+        <v>13</v>
+      </c>
+      <c r="C831" t="s">
+        <v>14</v>
+      </c>
+      <c r="D831">
+        <v>5</v>
+      </c>
+      <c r="E831" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="832" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A832" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B832" t="s">
+        <v>16</v>
+      </c>
+      <c r="C832" t="s">
+        <v>5</v>
+      </c>
+      <c r="D832">
+        <v>2</v>
+      </c>
+      <c r="E832" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="833" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A833" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B833" t="s">
+        <v>18</v>
+      </c>
+      <c r="C833" t="s">
+        <v>19</v>
+      </c>
+      <c r="D833">
+        <v>5</v>
+      </c>
+      <c r="E833" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="834" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A834" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B834" t="s">
+        <v>21</v>
+      </c>
+      <c r="C834" t="s">
+        <v>14</v>
+      </c>
+      <c r="D834">
+        <v>2</v>
+      </c>
+      <c r="E834" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="835" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A835" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B835" t="s">
+        <v>23</v>
+      </c>
+      <c r="C835" t="s">
+        <v>24</v>
+      </c>
+      <c r="D835">
+        <v>3</v>
+      </c>
+      <c r="E835" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="836" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A836" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B836" t="s">
+        <v>26</v>
+      </c>
+      <c r="C836" t="s">
+        <v>27</v>
+      </c>
+      <c r="D836">
+        <v>3</v>
+      </c>
+      <c r="E836" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="837" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A837" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B837" t="s">
+        <v>529</v>
+      </c>
+      <c r="C837" t="s">
+        <v>62</v>
+      </c>
+      <c r="D837">
+        <v>2</v>
+      </c>
+      <c r="E837" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="838" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A838" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B838" t="s">
+        <v>29</v>
+      </c>
+      <c r="C838" t="s">
+        <v>14</v>
+      </c>
+      <c r="D838">
+        <v>5</v>
+      </c>
+      <c r="E838" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="839" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A839" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B839" t="s">
+        <v>31</v>
+      </c>
+      <c r="C839" t="s">
+        <v>5</v>
+      </c>
+      <c r="D839">
+        <v>5</v>
+      </c>
+      <c r="E839" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="840" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A840" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B840" t="s">
+        <v>33</v>
+      </c>
+      <c r="C840" t="s">
+        <v>5</v>
+      </c>
+      <c r="D840">
+        <v>5</v>
+      </c>
+      <c r="E840" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="841" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A841" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B841" t="s">
+        <v>35</v>
+      </c>
+      <c r="C841" t="s">
+        <v>27</v>
+      </c>
+      <c r="D841">
+        <v>2</v>
+      </c>
+      <c r="E841" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="842" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A842" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B842" t="s">
+        <v>37</v>
+      </c>
+      <c r="C842" t="s">
+        <v>14</v>
+      </c>
+      <c r="D842">
+        <v>3</v>
+      </c>
+      <c r="E842" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="843" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A843" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B843" t="s">
+        <v>39</v>
+      </c>
+      <c r="C843" t="s">
+        <v>5</v>
+      </c>
+      <c r="D843">
+        <v>2</v>
+      </c>
+      <c r="E843" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="844" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A844" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B844" t="s">
+        <v>40</v>
+      </c>
+      <c r="C844" t="s">
+        <v>14</v>
+      </c>
+      <c r="D844">
+        <v>2</v>
+      </c>
+      <c r="E844" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="845" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A845" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B845" t="s">
+        <v>43</v>
+      </c>
+      <c r="C845" t="s">
+        <v>19</v>
+      </c>
+      <c r="D845">
+        <v>4</v>
+      </c>
+      <c r="E845" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="846" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A846" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B846" t="s">
+        <v>534</v>
+      </c>
+      <c r="C846" t="s">
+        <v>51</v>
+      </c>
+      <c r="D846">
+        <v>3</v>
+      </c>
+      <c r="E846" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="847" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A847" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B847" t="s">
+        <v>45</v>
+      </c>
+      <c r="C847" t="s">
+        <v>24</v>
+      </c>
+      <c r="D847">
+        <v>5</v>
+      </c>
+      <c r="E847" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="848" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A848" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B848" t="s">
+        <v>461</v>
+      </c>
+      <c r="C848" t="s">
+        <v>14</v>
+      </c>
+      <c r="D848">
+        <v>4</v>
+      </c>
+      <c r="E848" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="849" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A849" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B849" t="s">
+        <v>47</v>
+      </c>
+      <c r="C849" t="s">
+        <v>27</v>
+      </c>
+      <c r="D849">
+        <v>3</v>
+      </c>
+      <c r="E849" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="850" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A850" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B850" t="s">
+        <v>48</v>
+      </c>
+      <c r="C850" t="s">
+        <v>24</v>
+      </c>
+      <c r="D850">
+        <v>2</v>
+      </c>
+      <c r="E850" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="851" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A851" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B851" t="s">
+        <v>50</v>
+      </c>
+      <c r="C851" t="s">
+        <v>24</v>
+      </c>
+      <c r="D851">
+        <v>5</v>
+      </c>
+      <c r="E851" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="852" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A852" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B852" t="s">
+        <v>53</v>
+      </c>
+      <c r="C852" t="s">
+        <v>24</v>
+      </c>
+      <c r="D852">
+        <v>2</v>
+      </c>
+      <c r="E852" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="853" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A853" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B853" t="s">
+        <v>55</v>
+      </c>
+      <c r="C853" t="s">
+        <v>27</v>
+      </c>
+      <c r="D853">
+        <v>2</v>
+      </c>
+      <c r="E853" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="854" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A854" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B854" t="s">
+        <v>57</v>
+      </c>
+      <c r="C854" t="s">
+        <v>24</v>
+      </c>
+      <c r="D854">
+        <v>2</v>
+      </c>
+      <c r="E854" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="855" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A855" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B855" t="s">
+        <v>465</v>
+      </c>
+      <c r="C855" t="s">
+        <v>51</v>
+      </c>
+      <c r="D855">
+        <v>5</v>
+      </c>
+      <c r="E855" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="856" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A856" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B856" t="s">
+        <v>58</v>
+      </c>
+      <c r="C856" t="s">
+        <v>27</v>
+      </c>
+      <c r="D856">
+        <v>5</v>
+      </c>
+      <c r="E856" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="857" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A857" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B857" t="s">
+        <v>59</v>
+      </c>
+      <c r="C857" t="s">
+        <v>9</v>
+      </c>
+      <c r="D857">
+        <v>3</v>
+      </c>
+      <c r="E857" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="858" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A858" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B858" t="s">
+        <v>61</v>
+      </c>
+      <c r="C858" t="s">
+        <v>19</v>
+      </c>
+      <c r="D858">
+        <v>2</v>
+      </c>
+      <c r="E858" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="859" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A859" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B859" t="s">
+        <v>64</v>
+      </c>
+      <c r="C859" t="s">
+        <v>14</v>
+      </c>
+      <c r="D859">
+        <v>2</v>
+      </c>
+      <c r="E859" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="860" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A860" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B860" t="s">
+        <v>65</v>
+      </c>
+      <c r="C860" t="s">
+        <v>5</v>
+      </c>
+      <c r="D860">
+        <v>3</v>
+      </c>
+      <c r="E860" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="861" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A861" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B861" t="s">
+        <v>67</v>
+      </c>
+      <c r="C861" t="s">
+        <v>14</v>
+      </c>
+      <c r="D861">
+        <v>5</v>
+      </c>
+      <c r="E861" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="862" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A862" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B862" t="s">
+        <v>69</v>
+      </c>
+      <c r="C862" t="s">
+        <v>9</v>
+      </c>
+      <c r="D862">
+        <v>1</v>
+      </c>
+      <c r="E862" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="863" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A863" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B863" t="s">
+        <v>71</v>
+      </c>
+      <c r="C863" t="s">
+        <v>24</v>
+      </c>
+      <c r="D863">
+        <v>2</v>
+      </c>
+      <c r="E863" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="864" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A864" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B864" t="s">
+        <v>73</v>
+      </c>
+      <c r="C864" t="s">
+        <v>5</v>
+      </c>
+      <c r="D864">
+        <v>5</v>
+      </c>
+      <c r="E864" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="865" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A865" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B865" t="s">
+        <v>541</v>
+      </c>
+      <c r="C865" t="s">
+        <v>51</v>
+      </c>
+      <c r="D865">
+        <v>3</v>
+      </c>
+      <c r="E865" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="866" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A866" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B866" t="s">
+        <v>76</v>
+      </c>
+      <c r="C866" t="s">
+        <v>24</v>
+      </c>
+      <c r="D866">
+        <v>2</v>
+      </c>
+      <c r="E866" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="867" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A867" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B867" t="s">
+        <v>471</v>
+      </c>
+      <c r="C867" t="s">
+        <v>62</v>
+      </c>
+      <c r="D867">
+        <v>3</v>
+      </c>
+      <c r="E867" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="868" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A868" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B868" t="s">
+        <v>78</v>
+      </c>
+      <c r="C868" t="s">
+        <v>27</v>
+      </c>
+      <c r="D868">
+        <v>2</v>
+      </c>
+      <c r="E868" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="869" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A869" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B869" t="s">
+        <v>79</v>
+      </c>
+      <c r="C869" t="s">
+        <v>14</v>
+      </c>
+      <c r="D869">
+        <v>2</v>
+      </c>
+      <c r="E869" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="870" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A870" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B870" t="s">
+        <v>80</v>
+      </c>
+      <c r="C870" t="s">
+        <v>27</v>
+      </c>
+      <c r="D870">
+        <v>5</v>
+      </c>
+      <c r="E870" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="871" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A871" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B871" t="s">
+        <v>82</v>
+      </c>
+      <c r="C871" t="s">
+        <v>9</v>
+      </c>
+      <c r="D871">
+        <v>5</v>
+      </c>
+      <c r="E871" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="872" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A872" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B872" t="s">
+        <v>84</v>
+      </c>
+      <c r="C872" t="s">
+        <v>9</v>
+      </c>
+      <c r="D872">
+        <v>5</v>
+      </c>
+      <c r="E872" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="873" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A873" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B873" t="s">
+        <v>86</v>
+      </c>
+      <c r="C873" t="s">
+        <v>9</v>
+      </c>
+      <c r="D873">
+        <v>2</v>
+      </c>
+      <c r="E873" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="874" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A874" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B874" t="s">
+        <v>88</v>
+      </c>
+      <c r="C874" t="s">
+        <v>5</v>
+      </c>
+      <c r="D874">
+        <v>2</v>
+      </c>
+      <c r="E874" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="875" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A875" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B875" t="s">
+        <v>92</v>
+      </c>
+      <c r="C875" t="s">
+        <v>24</v>
+      </c>
+      <c r="D875">
+        <v>4</v>
+      </c>
+      <c r="E875" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="876" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A876" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B876" t="s">
+        <v>94</v>
+      </c>
+      <c r="C876" t="s">
+        <v>24</v>
+      </c>
+      <c r="D876">
+        <v>5</v>
+      </c>
+      <c r="E876" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="877" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A877" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B877" t="s">
+        <v>96</v>
+      </c>
+      <c r="C877" t="s">
+        <v>27</v>
+      </c>
+      <c r="D877">
+        <v>2</v>
+      </c>
+      <c r="E877" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="878" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A878" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B878" t="s">
+        <v>98</v>
+      </c>
+      <c r="C878" t="s">
+        <v>9</v>
+      </c>
+      <c r="D878">
+        <v>4</v>
+      </c>
+      <c r="E878" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="879" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A879" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B879" t="s">
+        <v>100</v>
+      </c>
+      <c r="C879" t="s">
+        <v>14</v>
+      </c>
+      <c r="D879">
+        <v>5</v>
+      </c>
+      <c r="E879" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="880" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A880" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B880" t="s">
+        <v>102</v>
+      </c>
+      <c r="C880" t="s">
+        <v>9</v>
+      </c>
+      <c r="D880">
+        <v>3</v>
+      </c>
+      <c r="E880" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="881" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A881" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B881" t="s">
+        <v>104</v>
+      </c>
+      <c r="C881" t="s">
+        <v>19</v>
+      </c>
+      <c r="D881">
+        <v>2</v>
+      </c>
+      <c r="E881" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="882" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A882" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B882" t="s">
+        <v>544</v>
+      </c>
+      <c r="C882" t="s">
+        <v>62</v>
+      </c>
+      <c r="D882">
+        <v>3</v>
+      </c>
+      <c r="E882" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="883" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A883" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B883" t="s">
+        <v>105</v>
+      </c>
+      <c r="C883" t="s">
+        <v>14</v>
+      </c>
+      <c r="D883">
+        <v>3</v>
+      </c>
+      <c r="E883" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="884" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A884" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B884" t="s">
+        <v>107</v>
+      </c>
+      <c r="C884" t="s">
+        <v>5</v>
+      </c>
+      <c r="D884">
+        <v>3</v>
+      </c>
+      <c r="E884" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="885" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A885" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B885" t="s">
+        <v>108</v>
+      </c>
+      <c r="C885" t="s">
+        <v>5</v>
+      </c>
+      <c r="D885">
+        <v>5</v>
+      </c>
+      <c r="E885" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="886" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A886" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B886" t="s">
+        <v>109</v>
+      </c>
+      <c r="C886" t="s">
+        <v>24</v>
+      </c>
+      <c r="D886">
+        <v>3</v>
+      </c>
+      <c r="E886" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="887" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A887" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B887" t="s">
+        <v>111</v>
+      </c>
+      <c r="C887" t="s">
+        <v>5</v>
+      </c>
+      <c r="D887">
+        <v>4</v>
+      </c>
+      <c r="E887" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="888" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A888" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B888" t="s">
+        <v>112</v>
+      </c>
+      <c r="C888" t="s">
+        <v>5</v>
+      </c>
+      <c r="D888">
+        <v>2</v>
+      </c>
+      <c r="E888" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="889" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A889" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B889" t="s">
+        <v>114</v>
+      </c>
+      <c r="C889" t="s">
+        <v>9</v>
+      </c>
+      <c r="D889">
+        <v>2</v>
+      </c>
+      <c r="E889" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="890" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A890" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B890" t="s">
+        <v>115</v>
+      </c>
+      <c r="C890" t="s">
+        <v>9</v>
+      </c>
+      <c r="D890">
+        <v>3</v>
+      </c>
+      <c r="E890" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="891" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A891" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B891" t="s">
+        <v>116</v>
+      </c>
+      <c r="C891" t="s">
+        <v>5</v>
+      </c>
+      <c r="D891">
+        <v>2</v>
+      </c>
+      <c r="E891" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="892" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A892" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B892" t="s">
+        <v>117</v>
+      </c>
+      <c r="C892" t="s">
+        <v>14</v>
+      </c>
+      <c r="D892">
+        <v>4</v>
+      </c>
+      <c r="E892" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="893" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A893" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B893" t="s">
+        <v>118</v>
+      </c>
+      <c r="C893" t="s">
+        <v>24</v>
+      </c>
+      <c r="D893">
+        <v>1</v>
+      </c>
+      <c r="E893" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="894" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A894" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B894" t="s">
+        <v>120</v>
+      </c>
+      <c r="C894" t="s">
+        <v>24</v>
+      </c>
+      <c r="D894">
+        <v>5</v>
+      </c>
+      <c r="E894" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="895" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A895" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B895" t="s">
+        <v>122</v>
+      </c>
+      <c r="C895" t="s">
+        <v>14</v>
+      </c>
+      <c r="D895">
+        <v>2</v>
+      </c>
+      <c r="E895" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="896" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A896" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B896" t="s">
+        <v>126</v>
+      </c>
+      <c r="C896" t="s">
+        <v>24</v>
+      </c>
+      <c r="D896">
+        <v>5</v>
+      </c>
+      <c r="E896" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="897" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A897" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B897" t="s">
+        <v>127</v>
+      </c>
+      <c r="C897" t="s">
+        <v>9</v>
+      </c>
+      <c r="D897">
+        <v>2</v>
+      </c>
+      <c r="E897" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="898" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A898" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B898" t="s">
+        <v>129</v>
+      </c>
+      <c r="C898" t="s">
+        <v>19</v>
+      </c>
+      <c r="D898">
+        <v>3</v>
+      </c>
+      <c r="E898" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="899" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A899" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B899" t="s">
+        <v>131</v>
+      </c>
+      <c r="C899" t="s">
+        <v>5</v>
+      </c>
+      <c r="D899">
+        <v>5</v>
+      </c>
+      <c r="E899" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="900" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A900" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B900" t="s">
+        <v>132</v>
+      </c>
+      <c r="C900" t="s">
+        <v>19</v>
+      </c>
+      <c r="D900">
+        <v>2</v>
+      </c>
+      <c r="E900" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="901" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A901" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B901" t="s">
+        <v>133</v>
+      </c>
+      <c r="C901" t="s">
+        <v>5</v>
+      </c>
+      <c r="D901">
+        <v>4</v>
+      </c>
+      <c r="E901" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="902" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A902" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B902" t="s">
+        <v>134</v>
+      </c>
+      <c r="C902" t="s">
+        <v>5</v>
+      </c>
+      <c r="D902">
+        <v>2</v>
+      </c>
+      <c r="E902" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="903" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A903" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B903" t="s">
+        <v>136</v>
+      </c>
+      <c r="C903" t="s">
+        <v>14</v>
+      </c>
+      <c r="D903">
+        <v>5</v>
+      </c>
+      <c r="E903" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="904" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A904" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B904" t="s">
+        <v>141</v>
+      </c>
+      <c r="C904" t="s">
+        <v>27</v>
+      </c>
+      <c r="D904">
+        <v>2</v>
+      </c>
+      <c r="E904" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="905" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A905" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B905" t="s">
+        <v>142</v>
+      </c>
+      <c r="C905" t="s">
+        <v>14</v>
+      </c>
+      <c r="D905">
+        <v>3</v>
+      </c>
+      <c r="E905" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="906" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A906" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B906" t="s">
+        <v>143</v>
+      </c>
+      <c r="C906" t="s">
+        <v>5</v>
+      </c>
+      <c r="D906">
+        <v>2</v>
+      </c>
+      <c r="E906" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="907" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A907" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B907" t="s">
+        <v>144</v>
+      </c>
+      <c r="C907" t="s">
+        <v>9</v>
+      </c>
+      <c r="D907">
+        <v>3</v>
+      </c>
+      <c r="E907" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="908" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A908" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B908" t="s">
+        <v>145</v>
+      </c>
+      <c r="C908" t="s">
+        <v>5</v>
+      </c>
+      <c r="D908">
+        <v>4</v>
+      </c>
+      <c r="E908" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="909" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A909" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B909" t="s">
+        <v>146</v>
+      </c>
+      <c r="C909" t="s">
+        <v>5</v>
+      </c>
+      <c r="D909">
+        <v>5</v>
+      </c>
+      <c r="E909" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="910" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A910" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B910" t="s">
+        <v>147</v>
+      </c>
+      <c r="C910" t="s">
+        <v>9</v>
+      </c>
+      <c r="D910">
+        <v>5</v>
+      </c>
+      <c r="E910" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="911" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A911" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B911" t="s">
+        <v>148</v>
+      </c>
+      <c r="C911" t="s">
+        <v>5</v>
+      </c>
+      <c r="D911">
+        <v>3</v>
+      </c>
+      <c r="E911" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="912" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A912" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B912" t="s">
+        <v>149</v>
+      </c>
+      <c r="C912" t="s">
+        <v>5</v>
+      </c>
+      <c r="D912">
+        <v>3</v>
+      </c>
+      <c r="E912" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="913" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A913" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B913" t="s">
+        <v>150</v>
+      </c>
+      <c r="C913" t="s">
+        <v>27</v>
+      </c>
+      <c r="D913">
+        <v>4</v>
+      </c>
+      <c r="E913" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="914" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A914" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B914" t="s">
+        <v>152</v>
+      </c>
+      <c r="C914" t="s">
+        <v>14</v>
+      </c>
+      <c r="D914">
+        <v>5</v>
+      </c>
+      <c r="E914" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="915" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A915" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B915" t="s">
+        <v>154</v>
+      </c>
+      <c r="C915" t="s">
+        <v>9</v>
+      </c>
+      <c r="D915">
+        <v>5</v>
+      </c>
+      <c r="E915" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="916" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A916" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B916" t="s">
+        <v>156</v>
+      </c>
+      <c r="C916" t="s">
+        <v>14</v>
+      </c>
+      <c r="D916">
+        <v>3</v>
+      </c>
+      <c r="E916" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="917" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A917" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B917" t="s">
+        <v>157</v>
+      </c>
+      <c r="C917" t="s">
+        <v>14</v>
+      </c>
+      <c r="D917">
+        <v>3</v>
+      </c>
+      <c r="E917" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="918" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A918" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B918" t="s">
+        <v>158</v>
+      </c>
+      <c r="C918" t="s">
+        <v>9</v>
+      </c>
+      <c r="D918">
+        <v>2</v>
+      </c>
+      <c r="E918" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="919" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A919" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B919" t="s">
+        <v>159</v>
+      </c>
+      <c r="C919" t="s">
+        <v>24</v>
+      </c>
+      <c r="D919">
+        <v>2</v>
+      </c>
+      <c r="E919" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="920" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A920" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B920" t="s">
+        <v>160</v>
+      </c>
+      <c r="C920" t="s">
+        <v>14</v>
+      </c>
+      <c r="D920">
+        <v>2</v>
+      </c>
+      <c r="E920" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="921" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A921" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B921" t="s">
+        <v>485</v>
+      </c>
+      <c r="C921" t="s">
+        <v>5</v>
+      </c>
+      <c r="D921">
+        <v>5</v>
+      </c>
+      <c r="E921" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="922" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A922" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B922" t="s">
+        <v>161</v>
+      </c>
+      <c r="C922" t="s">
+        <v>14</v>
+      </c>
+      <c r="D922">
+        <v>2</v>
+      </c>
+      <c r="E922" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="923" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A923" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B923" t="s">
+        <v>557</v>
+      </c>
+      <c r="C923" t="s">
+        <v>51</v>
+      </c>
+      <c r="D923">
+        <v>3</v>
+      </c>
+      <c r="E923" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="924" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A924" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B924" t="s">
+        <v>164</v>
+      </c>
+      <c r="C924" t="s">
+        <v>24</v>
+      </c>
+      <c r="D924">
+        <v>5</v>
+      </c>
+      <c r="E924" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="925" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A925" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B925" t="s">
+        <v>165</v>
+      </c>
+      <c r="C925" t="s">
+        <v>5</v>
+      </c>
+      <c r="D925">
+        <v>2</v>
+      </c>
+      <c r="E925" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="926" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A926" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B926" t="s">
+        <v>166</v>
+      </c>
+      <c r="C926" t="s">
+        <v>19</v>
+      </c>
+      <c r="D926">
+        <v>3</v>
+      </c>
+      <c r="E926" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="927" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A927" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B927" t="s">
+        <v>168</v>
+      </c>
+      <c r="C927" t="s">
+        <v>5</v>
+      </c>
+      <c r="D927">
+        <v>2</v>
+      </c>
+      <c r="E927" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="928" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A928" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B928" t="s">
+        <v>169</v>
+      </c>
+      <c r="C928" t="s">
+        <v>19</v>
+      </c>
+      <c r="D928">
+        <v>5</v>
+      </c>
+      <c r="E928" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="929" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A929" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B929" t="s">
+        <v>170</v>
+      </c>
+      <c r="C929" t="s">
+        <v>14</v>
+      </c>
+      <c r="D929">
+        <v>2</v>
+      </c>
+      <c r="E929" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="930" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A930" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B930" t="s">
+        <v>171</v>
+      </c>
+      <c r="C930" t="s">
+        <v>24</v>
+      </c>
+      <c r="D930">
+        <v>3</v>
+      </c>
+      <c r="E930" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="931" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A931" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B931" t="s">
+        <v>173</v>
+      </c>
+      <c r="C931" t="s">
+        <v>14</v>
+      </c>
+      <c r="D931">
+        <v>1</v>
+      </c>
+      <c r="E931" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="932" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A932" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B932" t="s">
+        <v>559</v>
+      </c>
+      <c r="C932" t="s">
+        <v>51</v>
+      </c>
+      <c r="D932">
+        <v>2</v>
+      </c>
+      <c r="E932" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="933" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A933" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B933" t="s">
+        <v>174</v>
+      </c>
+      <c r="C933" t="s">
+        <v>19</v>
+      </c>
+      <c r="D933">
+        <v>3</v>
+      </c>
+      <c r="E933" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="934" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A934" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B934" t="s">
+        <v>176</v>
+      </c>
+      <c r="C934" t="s">
+        <v>9</v>
+      </c>
+      <c r="D934">
+        <v>3</v>
+      </c>
+      <c r="E934" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="935" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A935" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B935" t="s">
+        <v>178</v>
+      </c>
+      <c r="C935" t="s">
+        <v>27</v>
+      </c>
+      <c r="D935">
+        <v>1</v>
+      </c>
+      <c r="E935" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="936" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A936" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B936" t="s">
+        <v>179</v>
+      </c>
+      <c r="C936" t="s">
+        <v>14</v>
+      </c>
+      <c r="D936">
+        <v>2</v>
+      </c>
+      <c r="E936" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="937" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A937" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B937" t="s">
+        <v>560</v>
+      </c>
+      <c r="C937" t="s">
+        <v>62</v>
+      </c>
+      <c r="D937">
+        <v>3</v>
+      </c>
+      <c r="E937" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="938" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A938" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B938" t="s">
+        <v>181</v>
+      </c>
+      <c r="C938" t="s">
+        <v>14</v>
+      </c>
+      <c r="D938">
+        <v>5</v>
+      </c>
+      <c r="E938" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="939" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A939" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B939" t="s">
+        <v>182</v>
+      </c>
+      <c r="C939" t="s">
+        <v>27</v>
+      </c>
+      <c r="D939">
+        <v>4</v>
+      </c>
+      <c r="E939" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="940" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A940" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B940" t="s">
+        <v>184</v>
+      </c>
+      <c r="C940" t="s">
+        <v>24</v>
+      </c>
+      <c r="D940">
+        <v>4</v>
+      </c>
+      <c r="E940" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="941" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A941" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B941" t="s">
+        <v>186</v>
+      </c>
+      <c r="C941" t="s">
+        <v>9</v>
+      </c>
+      <c r="D941">
+        <v>2</v>
+      </c>
+      <c r="E941" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="942" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A942" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B942" t="s">
+        <v>187</v>
+      </c>
+      <c r="C942" t="s">
+        <v>14</v>
+      </c>
+      <c r="D942">
+        <v>4</v>
+      </c>
+      <c r="E942" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="943" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A943" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B943" t="s">
+        <v>189</v>
+      </c>
+      <c r="C943" t="s">
+        <v>5</v>
+      </c>
+      <c r="D943">
+        <v>2</v>
+      </c>
+      <c r="E943" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="944" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A944" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B944" t="s">
+        <v>191</v>
+      </c>
+      <c r="C944" t="s">
+        <v>19</v>
+      </c>
+      <c r="D944">
+        <v>5</v>
+      </c>
+      <c r="E944" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="945" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A945" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B945" t="s">
+        <v>192</v>
+      </c>
+      <c r="C945" t="s">
+        <v>27</v>
+      </c>
+      <c r="D945">
+        <v>4</v>
+      </c>
+      <c r="E945" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="946" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A946" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B946" t="s">
+        <v>194</v>
+      </c>
+      <c r="C946" t="s">
+        <v>5</v>
+      </c>
+      <c r="D946">
+        <v>3</v>
+      </c>
+      <c r="E946" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="947" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A947" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B947" t="s">
+        <v>195</v>
+      </c>
+      <c r="C947" t="s">
+        <v>24</v>
+      </c>
+      <c r="D947">
+        <v>2</v>
+      </c>
+      <c r="E947" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="948" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A948" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B948" t="s">
+        <v>196</v>
+      </c>
+      <c r="C948" t="s">
+        <v>9</v>
+      </c>
+      <c r="D948">
+        <v>4</v>
+      </c>
+      <c r="E948" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="949" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A949" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B949" t="s">
+        <v>197</v>
+      </c>
+      <c r="C949" t="s">
+        <v>5</v>
+      </c>
+      <c r="D949">
+        <v>2</v>
+      </c>
+      <c r="E949" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="950" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A950" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B950" t="s">
+        <v>198</v>
+      </c>
+      <c r="C950" t="s">
+        <v>14</v>
+      </c>
+      <c r="D950">
+        <v>2</v>
+      </c>
+      <c r="E950" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="951" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A951" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B951" t="s">
+        <v>202</v>
+      </c>
+      <c r="C951" t="s">
+        <v>24</v>
+      </c>
+      <c r="D951">
+        <v>3</v>
+      </c>
+      <c r="E951" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="952" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A952" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B952" t="s">
+        <v>204</v>
+      </c>
+      <c r="C952" t="s">
+        <v>19</v>
+      </c>
+      <c r="D952">
+        <v>4</v>
+      </c>
+      <c r="E952" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="953" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A953" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B953" t="s">
+        <v>205</v>
+      </c>
+      <c r="C953" t="s">
+        <v>24</v>
+      </c>
+      <c r="D953">
+        <v>2</v>
+      </c>
+      <c r="E953" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="954" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A954" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B954" t="s">
+        <v>207</v>
+      </c>
+      <c r="C954" t="s">
+        <v>14</v>
+      </c>
+      <c r="D954">
+        <v>1</v>
+      </c>
+      <c r="E954" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="955" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A955" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B955" t="s">
+        <v>209</v>
+      </c>
+      <c r="C955" t="s">
+        <v>14</v>
+      </c>
+      <c r="D955">
+        <v>5</v>
+      </c>
+      <c r="E955" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="956" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A956" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B956" t="s">
+        <v>211</v>
+      </c>
+      <c r="C956" t="s">
+        <v>27</v>
+      </c>
+      <c r="D956">
+        <v>5</v>
+      </c>
+      <c r="E956" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="957" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A957" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B957" t="s">
+        <v>212</v>
+      </c>
+      <c r="C957" t="s">
+        <v>9</v>
+      </c>
+      <c r="D957">
+        <v>2</v>
+      </c>
+      <c r="E957" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="958" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A958" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B958" t="s">
+        <v>213</v>
+      </c>
+      <c r="C958" t="s">
+        <v>5</v>
+      </c>
+      <c r="D958">
+        <v>2</v>
+      </c>
+      <c r="E958" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="959" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A959" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B959" t="s">
+        <v>215</v>
+      </c>
+      <c r="C959" t="s">
+        <v>24</v>
+      </c>
+      <c r="D959">
+        <v>3</v>
+      </c>
+      <c r="E959" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="960" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A960" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B960" t="s">
+        <v>216</v>
+      </c>
+      <c r="C960" t="s">
+        <v>24</v>
+      </c>
+      <c r="D960">
+        <v>3</v>
+      </c>
+      <c r="E960" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="961" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A961" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B961" t="s">
+        <v>572</v>
+      </c>
+      <c r="C961" t="s">
+        <v>51</v>
+      </c>
+      <c r="D961">
+        <v>2</v>
+      </c>
+      <c r="E961" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="962" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A962" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B962" t="s">
+        <v>218</v>
+      </c>
+      <c r="C962" t="s">
+        <v>5</v>
+      </c>
+      <c r="D962">
+        <v>5</v>
+      </c>
+      <c r="E962" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="963" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A963" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B963" t="s">
+        <v>220</v>
+      </c>
+      <c r="C963" t="s">
+        <v>24</v>
+      </c>
+      <c r="D963">
+        <v>2</v>
+      </c>
+      <c r="E963" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="964" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A964" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B964" t="s">
+        <v>222</v>
+      </c>
+      <c r="C964" t="s">
+        <v>24</v>
+      </c>
+      <c r="D964">
+        <v>4</v>
+      </c>
+      <c r="E964" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="965" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A965" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B965" t="s">
+        <v>223</v>
+      </c>
+      <c r="C965" t="s">
+        <v>27</v>
+      </c>
+      <c r="D965">
+        <v>2</v>
+      </c>
+      <c r="E965" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="966" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A966" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B966" t="s">
+        <v>224</v>
+      </c>
+      <c r="C966" t="s">
+        <v>5</v>
+      </c>
+      <c r="D966">
+        <v>3</v>
+      </c>
+      <c r="E966" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="967" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A967" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B967" t="s">
+        <v>225</v>
+      </c>
+      <c r="C967" t="s">
+        <v>9</v>
+      </c>
+      <c r="D967">
+        <v>3</v>
+      </c>
+      <c r="E967" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="968" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A968" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B968" t="s">
+        <v>226</v>
+      </c>
+      <c r="C968" t="s">
+        <v>9</v>
+      </c>
+      <c r="D968">
+        <v>2</v>
+      </c>
+      <c r="E968" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="969" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A969" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B969" t="s">
+        <v>229</v>
+      </c>
+      <c r="C969" t="s">
+        <v>9</v>
+      </c>
+      <c r="D969">
+        <v>2</v>
+      </c>
+      <c r="E969" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="970" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A970" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B970" t="s">
+        <v>231</v>
+      </c>
+      <c r="C970" t="s">
+        <v>24</v>
+      </c>
+      <c r="D970">
+        <v>5</v>
+      </c>
+      <c r="E970" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="971" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A971" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B971" t="s">
+        <v>233</v>
+      </c>
+      <c r="C971" t="s">
+        <v>5</v>
+      </c>
+      <c r="D971">
+        <v>2</v>
+      </c>
+      <c r="E971" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="972" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A972" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B972" t="s">
+        <v>234</v>
+      </c>
+      <c r="C972" t="s">
+        <v>5</v>
+      </c>
+      <c r="D972">
+        <v>3</v>
+      </c>
+      <c r="E972" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="973" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A973" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B973" t="s">
+        <v>577</v>
+      </c>
+      <c r="C973" t="s">
+        <v>62</v>
+      </c>
+      <c r="D973">
+        <v>3</v>
+      </c>
+      <c r="E973" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="974" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A974" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B974" t="s">
+        <v>235</v>
+      </c>
+      <c r="C974" t="s">
+        <v>9</v>
+      </c>
+      <c r="D974">
+        <v>5</v>
+      </c>
+      <c r="E974" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="975" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A975" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B975" t="s">
+        <v>236</v>
+      </c>
+      <c r="C975" t="s">
+        <v>14</v>
+      </c>
+      <c r="D975">
+        <v>3</v>
+      </c>
+      <c r="E975" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="976" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A976" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B976" t="s">
+        <v>237</v>
+      </c>
+      <c r="C976" t="s">
+        <v>9</v>
+      </c>
+      <c r="D976">
+        <v>5</v>
+      </c>
+      <c r="E976" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="977" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A977" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B977" t="s">
+        <v>238</v>
+      </c>
+      <c r="C977" t="s">
+        <v>14</v>
+      </c>
+      <c r="D977">
+        <v>2</v>
+      </c>
+      <c r="E977" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="978" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A978" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B978" t="s">
+        <v>239</v>
+      </c>
+      <c r="C978" t="s">
+        <v>9</v>
+      </c>
+      <c r="D978">
+        <v>5</v>
+      </c>
+      <c r="E978" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="979" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A979" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B979" t="s">
+        <v>240</v>
+      </c>
+      <c r="C979" t="s">
+        <v>14</v>
+      </c>
+      <c r="D979">
+        <v>2</v>
+      </c>
+      <c r="E979" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="980" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A980" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B980" t="s">
+        <v>242</v>
+      </c>
+      <c r="C980" t="s">
+        <v>24</v>
+      </c>
+      <c r="D980">
+        <v>3</v>
+      </c>
+      <c r="E980" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="981" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A981" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B981" t="s">
+        <v>244</v>
+      </c>
+      <c r="C981" t="s">
+        <v>9</v>
+      </c>
+      <c r="D981">
+        <v>5</v>
+      </c>
+      <c r="E981" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="982" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A982" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B982" t="s">
+        <v>245</v>
+      </c>
+      <c r="C982" t="s">
+        <v>5</v>
+      </c>
+      <c r="D982">
+        <v>5</v>
+      </c>
+      <c r="E982" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="983" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A983" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B983" t="s">
+        <v>247</v>
+      </c>
+      <c r="C983" t="s">
+        <v>5</v>
+      </c>
+      <c r="D983">
+        <v>5</v>
+      </c>
+      <c r="E983" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="984" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A984" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B984" t="s">
+        <v>248</v>
+      </c>
+      <c r="C984" t="s">
+        <v>27</v>
+      </c>
+      <c r="D984">
+        <v>5</v>
+      </c>
+      <c r="E984" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="985" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A985" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B985" t="s">
+        <v>250</v>
+      </c>
+      <c r="C985" t="s">
+        <v>24</v>
+      </c>
+      <c r="D985">
+        <v>5</v>
+      </c>
+      <c r="E985" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="986" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A986" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B986" t="s">
+        <v>252</v>
+      </c>
+      <c r="C986" t="s">
+        <v>9</v>
+      </c>
+      <c r="D986">
+        <v>2</v>
+      </c>
+      <c r="E986" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="987" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A987" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B987" t="s">
+        <v>253</v>
+      </c>
+      <c r="C987" t="s">
+        <v>24</v>
+      </c>
+      <c r="D987">
+        <v>4</v>
+      </c>
+      <c r="E987" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="988" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A988" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B988" t="s">
+        <v>255</v>
+      </c>
+      <c r="C988" t="s">
+        <v>9</v>
+      </c>
+      <c r="D988">
+        <v>3</v>
+      </c>
+      <c r="E988" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="989" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A989" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B989" t="s">
+        <v>257</v>
+      </c>
+      <c r="C989" t="s">
+        <v>14</v>
+      </c>
+      <c r="D989">
+        <v>3</v>
+      </c>
+      <c r="E989" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="990" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A990" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B990" t="s">
+        <v>258</v>
+      </c>
+      <c r="C990" t="s">
+        <v>14</v>
+      </c>
+      <c r="D990">
+        <v>2</v>
+      </c>
+      <c r="E990" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="991" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A991" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B991" t="s">
+        <v>585</v>
+      </c>
+      <c r="C991" t="s">
+        <v>62</v>
+      </c>
+      <c r="D991">
+        <v>2</v>
+      </c>
+      <c r="E991" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="992" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A992" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B992" t="s">
+        <v>260</v>
+      </c>
+      <c r="C992" t="s">
+        <v>9</v>
+      </c>
+      <c r="D992">
+        <v>3</v>
+      </c>
+      <c r="E992" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="993" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A993" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B993" t="s">
+        <v>261</v>
+      </c>
+      <c r="C993" t="s">
+        <v>5</v>
+      </c>
+      <c r="D993">
+        <v>3</v>
+      </c>
+      <c r="E993" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="994" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A994" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B994" t="s">
+        <v>262</v>
+      </c>
+      <c r="C994" t="s">
+        <v>24</v>
+      </c>
+      <c r="D994">
+        <v>5</v>
+      </c>
+      <c r="E994" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="995" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A995" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B995" t="s">
+        <v>263</v>
+      </c>
+      <c r="C995" t="s">
+        <v>24</v>
+      </c>
+      <c r="D995">
+        <v>5</v>
+      </c>
+      <c r="E995" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="996" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A996" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B996" t="s">
+        <v>264</v>
+      </c>
+      <c r="C996" t="s">
+        <v>9</v>
+      </c>
+      <c r="D996">
+        <v>2</v>
+      </c>
+      <c r="E996" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="997" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A997" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B997" t="s">
+        <v>265</v>
+      </c>
+      <c r="C997" t="s">
+        <v>9</v>
+      </c>
+      <c r="D997">
+        <v>4</v>
+      </c>
+      <c r="E997" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="998" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A998" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B998" t="s">
+        <v>267</v>
+      </c>
+      <c r="C998" t="s">
+        <v>24</v>
+      </c>
+      <c r="D998">
+        <v>5</v>
+      </c>
+      <c r="E998" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="999" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A999" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B999" t="s">
+        <v>269</v>
+      </c>
+      <c r="C999" t="s">
+        <v>5</v>
+      </c>
+      <c r="D999">
+        <v>2</v>
+      </c>
+      <c r="E999" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="1000" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1000" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B1000" t="s">
+        <v>270</v>
+      </c>
+      <c r="C1000" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1000">
+        <v>3</v>
+      </c>
+      <c r="E1000" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="1001" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1001" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B1001" t="s">
+        <v>271</v>
+      </c>
+      <c r="C1001" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1001">
+        <v>3</v>
+      </c>
+      <c r="E1001" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="1002" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1002" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B1002" t="s">
+        <v>272</v>
+      </c>
+      <c r="C1002" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1002">
+        <v>2</v>
+      </c>
+      <c r="E1002" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="1003" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1003" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B1003" t="s">
+        <v>273</v>
+      </c>
+      <c r="C1003" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1003">
+        <v>5</v>
+      </c>
+      <c r="E1003" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1004" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B1004" t="s">
+        <v>274</v>
+      </c>
+      <c r="C1004" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1004">
+        <v>5</v>
+      </c>
+      <c r="E1004" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1005" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B1005" t="s">
+        <v>275</v>
+      </c>
+      <c r="C1005" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1005">
+        <v>2</v>
+      </c>
+      <c r="E1005" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="1006" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1006" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B1006" t="s">
+        <v>276</v>
+      </c>
+      <c r="C1006" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1006">
+        <v>5</v>
+      </c>
+      <c r="E1006" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="1007" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1007" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B1007" t="s">
+        <v>277</v>
+      </c>
+      <c r="C1007" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1007">
+        <v>2</v>
+      </c>
+      <c r="E1007" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1008" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1008" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B1008" t="s">
+        <v>278</v>
+      </c>
+      <c r="C1008" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1008">
+        <v>5</v>
+      </c>
+      <c r="E1008" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="1009" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1009" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B1009" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1009" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1009">
+        <v>5</v>
+      </c>
+      <c r="E1009" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="1010" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1010" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B1010" t="s">
+        <v>280</v>
+      </c>
+      <c r="C1010" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1010">
+        <v>2</v>
+      </c>
+      <c r="E1010" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="1011" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1011" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B1011" t="s">
+        <v>512</v>
+      </c>
+      <c r="C1011" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1011">
+        <v>5</v>
+      </c>
+      <c r="E1011" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="1012" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1012" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B1012" t="s">
+        <v>281</v>
+      </c>
+      <c r="C1012" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1012">
+        <v>5</v>
+      </c>
+      <c r="E1012" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="1013" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1013" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B1013" t="s">
+        <v>282</v>
+      </c>
+      <c r="C1013" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1013">
+        <v>2</v>
+      </c>
+      <c r="E1013" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="1014" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1014" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B1014" t="s">
+        <v>283</v>
+      </c>
+      <c r="C1014" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1014">
+        <v>4</v>
+      </c>
+      <c r="E1014" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="1015" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1015" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B1015" t="s">
+        <v>284</v>
+      </c>
+      <c r="C1015" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1015">
+        <v>3</v>
+      </c>
+      <c r="E1015" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="1016" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1016" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B1016" t="s">
+        <v>285</v>
+      </c>
+      <c r="C1016" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1016">
+        <v>3</v>
+      </c>
+      <c r="E1016" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="1017" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1017" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B1017" t="s">
+        <v>286</v>
+      </c>
+      <c r="C1017" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1017">
+        <v>3</v>
+      </c>
+      <c r="E1017" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="1018" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1018" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B1018" t="s">
+        <v>288</v>
+      </c>
+      <c r="C1018" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1018">
+        <v>2</v>
+      </c>
+      <c r="E1018" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="1019" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1019" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B1019" t="s">
+        <v>289</v>
+      </c>
+      <c r="C1019" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1019">
+        <v>2</v>
+      </c>
+      <c r="E1019" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1020" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1020" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B1020" t="s">
+        <v>290</v>
+      </c>
+      <c r="C1020" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1020">
+        <v>5</v>
+      </c>
+      <c r="E1020" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="1021" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1021" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B1021" t="s">
+        <v>292</v>
+      </c>
+      <c r="C1021" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1021">
+        <v>5</v>
+      </c>
+      <c r="E1021" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="1022" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1022" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B1022" t="s">
+        <v>294</v>
+      </c>
+      <c r="C1022" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1022">
+        <v>1</v>
+      </c>
+      <c r="E1022" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1023" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1023" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B1023" t="s">
+        <v>295</v>
+      </c>
+      <c r="C1023" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1023">
+        <v>3</v>
+      </c>
+      <c r="E1023" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="1024" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1024" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B1024" t="s">
+        <v>297</v>
+      </c>
+      <c r="C1024" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1024">
+        <v>2</v>
+      </c>
+      <c r="E1024" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1025" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1025" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B1025" t="s">
+        <v>298</v>
+      </c>
+      <c r="C1025" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1025">
+        <v>3</v>
+      </c>
+      <c r="E1025" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="1026" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1026" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B1026" t="s">
+        <v>299</v>
+      </c>
+      <c r="C1026" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1026">
+        <v>2</v>
+      </c>
+      <c r="E1026" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1027" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1027" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B1027" t="s">
+        <v>300</v>
+      </c>
+      <c r="C1027" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1027">
+        <v>5</v>
+      </c>
+      <c r="E1027" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="1028" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1028" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B1028" t="s">
+        <v>302</v>
+      </c>
+      <c r="C1028" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1028">
+        <v>5</v>
+      </c>
+      <c r="E1028" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="1029" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1029" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B1029" t="s">
+        <v>304</v>
+      </c>
+      <c r="C1029" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1029">
+        <v>3</v>
+      </c>
+      <c r="E1029" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="1030" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1030" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B1030" t="s">
+        <v>521</v>
+      </c>
+      <c r="C1030" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1030">
+        <v>3</v>
+      </c>
+      <c r="E1030" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="1031" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1031" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B1031" t="s">
+        <v>306</v>
+      </c>
+      <c r="C1031" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1031">
+        <v>2</v>
+      </c>
+      <c r="E1031" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1032" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1032" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B1032" t="s">
+        <v>308</v>
+      </c>
+      <c r="C1032" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1032">
+        <v>3</v>
+      </c>
+      <c r="E1032" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="1033" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1033" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B1033" t="s">
+        <v>310</v>
+      </c>
+      <c r="C1033" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1033">
+        <v>2</v>
+      </c>
+      <c r="E1033" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1034" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1034" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B1034" t="s">
+        <v>311</v>
+      </c>
+      <c r="C1034" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1034">
+        <v>3</v>
+      </c>
+      <c r="E1034" t="s">
+        <v>600</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>